<commit_message>
25 temmuz sevkler işlendi
</commit_message>
<xml_diff>
--- a/Muhasebe.xlsx
+++ b/Muhasebe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BELEVİ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18B3183-432F-4628-BFC1-F3F3642624F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF11AA-2303-49F5-9C82-80D204606329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" activeTab="1" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GÜNLÜK_GELEN_GİDEN_MAL" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="271">
   <si>
     <t>MÜSTAHSİL</t>
   </si>
@@ -774,12 +774,6 @@
     <t>Genel Toplam</t>
   </si>
   <si>
-    <t>Değişen Toplam</t>
-  </si>
-  <si>
-    <t>Say</t>
-  </si>
-  <si>
     <t>Ünalberk</t>
   </si>
   <si>
@@ -841,6 +835,27 @@
   </si>
   <si>
     <t>ÖDEME</t>
+  </si>
+  <si>
+    <t>Sinan Küçükzeybek</t>
+  </si>
+  <si>
+    <t>25.7.2021/PAZAR</t>
+  </si>
+  <si>
+    <t>Ali Durmaz</t>
+  </si>
+  <si>
+    <t>Sedat Ektiren</t>
+  </si>
+  <si>
+    <t>ALİ DURMAZ</t>
+  </si>
+  <si>
+    <t>SEDAT EKTİREN</t>
+  </si>
+  <si>
+    <t>HAFTALIK TOPLAM</t>
   </si>
 </sst>
 </file>
@@ -1042,28 +1057,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1075,15 +1089,16 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1092,10 +1107,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1412,13 +1427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BD046-FBF6-4454-99AD-0B843F600705}">
-  <dimension ref="A1:BQ408"/>
+  <dimension ref="A1:BQ419"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B376" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B395" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O393" sqref="O393"/>
+      <selection pane="bottomRight" activeCell="BP418" sqref="BP418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1426,6 +1441,7 @@
     <col min="1" max="1" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.36328125" bestFit="1" customWidth="1"/>
@@ -1487,90 +1503,90 @@
         <v>171</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="31" t="s">
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="30" t="s">
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="39" t="s">
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="38" t="s">
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="37" t="s">
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="36" t="s">
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="AS1" s="36"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="36"/>
-      <c r="AV1" s="35" t="s">
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35"/>
+      <c r="AV1" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="AW1" s="35"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="35"/>
-      <c r="AZ1" s="31" t="s">
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="32" t="s">
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
-      <c r="BG1" s="32"/>
-      <c r="BH1" s="33" t="s">
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37"/>
+      <c r="BG1" s="37"/>
+      <c r="BH1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="34" t="s">
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="31"/>
+      <c r="BL1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
       <c r="BP1" s="2" t="s">
         <v>82</v>
       </c>
@@ -32181,7 +32197,7 @@
         <v>163</v>
       </c>
       <c r="C394" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D394">
         <v>783</v>
@@ -32321,7 +32337,7 @@
         <v>18862.5</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A401" s="2" t="s">
         <v>233</v>
       </c>
@@ -32349,7 +32365,7 @@
         <v>21997.8</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A402" s="2" t="s">
         <v>233</v>
       </c>
@@ -32377,7 +32393,7 @@
         <v>8190</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A403" s="2" t="s">
         <v>233</v>
       </c>
@@ -32405,7 +32421,7 @@
         <v>10600</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A404" s="2" t="s">
         <v>233</v>
       </c>
@@ -32436,7 +32452,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A405" s="2" t="s">
         <v>233</v>
       </c>
@@ -32464,7 +32480,7 @@
         <v>24786</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A406" s="2" t="s">
         <v>233</v>
       </c>
@@ -32492,7 +32508,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B407" s="2" t="s">
         <v>17</v>
       </c>
@@ -32518,7 +32534,7 @@
         <v>98036.3</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B408" s="2" t="s">
         <v>18</v>
       </c>
@@ -32527,13 +32543,258 @@
         <v>6.8442857142857134</v>
       </c>
     </row>
+    <row r="409" spans="1:60" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A409" s="10"/>
+    </row>
+    <row r="411" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A411" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B411" t="s">
+        <v>264</v>
+      </c>
+      <c r="D411">
+        <v>486</v>
+      </c>
+      <c r="E411">
+        <v>1860</v>
+      </c>
+      <c r="F411">
+        <v>240</v>
+      </c>
+      <c r="G411">
+        <f t="shared" ref="G411:G417" si="89">(E411-F411)</f>
+        <v>1620</v>
+      </c>
+      <c r="H411">
+        <v>7.22</v>
+      </c>
+      <c r="I411">
+        <f t="shared" ref="I411:I417" si="90">(G411*H411)</f>
+        <v>11696.4</v>
+      </c>
+      <c r="BD411">
+        <v>481</v>
+      </c>
+      <c r="BH411">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="412" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A412" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B412" t="s">
+        <v>266</v>
+      </c>
+      <c r="D412">
+        <v>48</v>
+      </c>
+      <c r="E412">
+        <v>280</v>
+      </c>
+      <c r="F412">
+        <v>48</v>
+      </c>
+      <c r="G412">
+        <f t="shared" si="89"/>
+        <v>232</v>
+      </c>
+      <c r="H412">
+        <v>7</v>
+      </c>
+      <c r="I412">
+        <f t="shared" si="90"/>
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="413" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A413" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B413" t="s">
+        <v>14</v>
+      </c>
+      <c r="D413">
+        <v>281</v>
+      </c>
+      <c r="E413">
+        <v>1860</v>
+      </c>
+      <c r="F413">
+        <v>281</v>
+      </c>
+      <c r="G413">
+        <f t="shared" si="89"/>
+        <v>1579</v>
+      </c>
+      <c r="H413">
+        <v>7.5</v>
+      </c>
+      <c r="I413">
+        <f t="shared" si="90"/>
+        <v>11842.5</v>
+      </c>
+    </row>
+    <row r="414" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A414" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B414" t="s">
+        <v>267</v>
+      </c>
+      <c r="D414">
+        <v>759</v>
+      </c>
+      <c r="E414">
+        <v>3300</v>
+      </c>
+      <c r="F414">
+        <v>300</v>
+      </c>
+      <c r="G414">
+        <f t="shared" si="89"/>
+        <v>3000</v>
+      </c>
+      <c r="H414">
+        <v>7.3</v>
+      </c>
+      <c r="I414">
+        <f t="shared" si="90"/>
+        <v>21900</v>
+      </c>
+    </row>
+    <row r="415" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A415" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B415" t="s">
+        <v>124</v>
+      </c>
+      <c r="D415">
+        <v>172</v>
+      </c>
+      <c r="E415">
+        <v>800</v>
+      </c>
+      <c r="F415">
+        <v>70</v>
+      </c>
+      <c r="G415">
+        <f t="shared" si="89"/>
+        <v>730</v>
+      </c>
+      <c r="H415">
+        <v>7.5</v>
+      </c>
+      <c r="I415">
+        <f t="shared" si="90"/>
+        <v>5475</v>
+      </c>
+    </row>
+    <row r="416" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A416" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B416" t="s">
+        <v>124</v>
+      </c>
+      <c r="D416">
+        <v>90</v>
+      </c>
+      <c r="E416">
+        <v>600</v>
+      </c>
+      <c r="F416">
+        <v>40</v>
+      </c>
+      <c r="G416">
+        <f t="shared" si="89"/>
+        <v>560</v>
+      </c>
+      <c r="H416">
+        <v>6</v>
+      </c>
+      <c r="I416">
+        <f t="shared" si="90"/>
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="417" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A417" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B417" t="s">
+        <v>8</v>
+      </c>
+      <c r="D417">
+        <v>591</v>
+      </c>
+      <c r="E417">
+        <v>2360</v>
+      </c>
+      <c r="F417">
+        <v>240</v>
+      </c>
+      <c r="G417">
+        <f t="shared" si="89"/>
+        <v>2120</v>
+      </c>
+      <c r="H417" s="6">
+        <v>7.27</v>
+      </c>
+      <c r="I417">
+        <f t="shared" si="90"/>
+        <v>15412.4</v>
+      </c>
+    </row>
+    <row r="418" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="B418" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D418" s="2">
+        <f t="shared" ref="D418:I418" si="91">SUM(D411:D417)</f>
+        <v>2427</v>
+      </c>
+      <c r="E418" s="2">
+        <f t="shared" si="91"/>
+        <v>11060</v>
+      </c>
+      <c r="F418" s="2">
+        <f t="shared" si="91"/>
+        <v>1219</v>
+      </c>
+      <c r="G418" s="2">
+        <f t="shared" si="91"/>
+        <v>9841</v>
+      </c>
+      <c r="H418" s="2"/>
+      <c r="I418" s="2">
+        <f t="shared" si="91"/>
+        <v>71310.3</v>
+      </c>
+      <c r="BD418" s="2">
+        <v>481</v>
+      </c>
+      <c r="BH418" s="2">
+        <v>1940</v>
+      </c>
+      <c r="BP418" s="2">
+        <f>(BD418+BH418)</f>
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="419" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="B419" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H419" s="2">
+        <f>AVERAGE(H411:H417)</f>
+        <v>7.1128571428571421</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="BH1:BK1"/>
-    <mergeCell ref="BL1:BO1"/>
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="X1:AA1"/>
@@ -32543,6 +32804,11 @@
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="BH1:BK1"/>
+    <mergeCell ref="BL1:BO1"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AR1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32625,14 +32891,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD1A8C-99DF-4166-8097-144C71FF7489}">
-  <dimension ref="A1:BL6"/>
+  <dimension ref="A1:BQ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="BH1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
@@ -32642,97 +32909,108 @@
     <col min="46" max="46" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="28"/>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="42" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
       <c r="O1" s="27"/>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="U1" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Z1" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="U1" s="39" t="s">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AE1" s="44" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Z1" s="34" t="s">
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AJ1" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AE1" s="42" t="s">
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AO1" s="45" t="s">
         <v>258</v>
-      </c>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AJ1" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AO1" s="45" t="s">
-        <v>260</v>
       </c>
       <c r="AP1" s="45"/>
       <c r="AQ1" s="45"/>
       <c r="AR1" s="45"/>
       <c r="AT1" s="46" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46"/>
       <c r="AW1" s="46"/>
-      <c r="AY1" s="47" t="s">
-        <v>262</v>
-      </c>
-      <c r="AZ1" s="47"/>
-      <c r="BA1" s="47"/>
-      <c r="BB1" s="47"/>
-      <c r="BD1" s="48" t="s">
-        <v>263</v>
-      </c>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
-      <c r="BL1" s="29"/>
-    </row>
-    <row r="2" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AY1" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ1" s="42"/>
+      <c r="BA1" s="42"/>
+      <c r="BB1" s="42"/>
+      <c r="BD1" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE1" s="43"/>
+      <c r="BF1" s="43"/>
+      <c r="BG1" s="43"/>
+      <c r="BI1" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BN1" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
+      <c r="BQ1" s="35"/>
+    </row>
+    <row r="2" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>234</v>
@@ -32741,10 +33019,10 @@
         <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>234</v>
@@ -32753,10 +33031,10 @@
         <v>59</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>234</v>
@@ -32765,10 +33043,10 @@
         <v>59</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>234</v>
@@ -32777,10 +33055,10 @@
         <v>59</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>234</v>
@@ -32789,10 +33067,10 @@
         <v>59</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>234</v>
@@ -32801,10 +33079,10 @@
         <v>59</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>234</v>
@@ -32813,10 +33091,10 @@
         <v>59</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AM2" s="2" t="s">
         <v>234</v>
@@ -32825,10 +33103,10 @@
         <v>59</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>234</v>
@@ -32837,10 +33115,10 @@
         <v>59</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>234</v>
@@ -32849,10 +33127,10 @@
         <v>59</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BB2" s="2" t="s">
         <v>234</v>
@@ -32861,16 +33139,40 @@
         <v>59</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BG2" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BI2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>38000</v>
       </c>
@@ -32995,8 +33297,41 @@
         <f>(BE3-BF3)</f>
         <v>7110</v>
       </c>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BI3" s="1">
+        <v>44402</v>
+      </c>
+      <c r="BJ3">
+        <v>1624</v>
+      </c>
+      <c r="BL3">
+        <f>(BJ3-BK3)</f>
+        <v>1624</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>44402</v>
+      </c>
+      <c r="BO3">
+        <v>21925</v>
+      </c>
+      <c r="BQ3">
+        <f>(BO3-BP3)</f>
+        <v>21925</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>44402</v>
+      </c>
+      <c r="B4">
+        <v>15400</v>
+      </c>
+      <c r="C4">
+        <v>33000</v>
+      </c>
+      <c r="D4">
+        <f>(B4-C4+D3)</f>
+        <v>20400</v>
+      </c>
       <c r="F4" s="1">
         <v>44399</v>
       </c>
@@ -33026,7 +33361,7 @@
       </c>
       <c r="AY4" s="1"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.35">
       <c r="F5" s="1">
         <v>44400</v>
       </c>
@@ -33052,24 +33387,47 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
-      <c r="K6" s="1"/>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="F6" s="1">
+        <v>44402</v>
+      </c>
+      <c r="G6">
+        <v>11840</v>
+      </c>
+      <c r="I6">
+        <f>(G6-H6+I5)</f>
+        <v>87792</v>
+      </c>
+      <c r="K6" s="1">
+        <v>44402</v>
+      </c>
+      <c r="L6">
+        <v>8835</v>
+      </c>
+      <c r="M6">
+        <v>19500</v>
+      </c>
+      <c r="N6">
+        <f>(L6-M6+N5)</f>
+        <v>31093</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BD1:BG1"/>
-    <mergeCell ref="BI1:BL1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="BI1:BL1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BD1:BG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33077,10 +33435,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F781AA57-6247-4A4F-9752-70CC607DC978}">
-  <dimension ref="A1:AK95"/>
+  <dimension ref="A1:AK98"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView topLeftCell="A66" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="K103" sqref="K103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33109,21 +33467,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -33337,36 +33695,36 @@
     </row>
     <row r="11" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29" t="s">
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29" t="s">
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29" t="s">
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29" t="s">
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
       <c r="Z12" s="25" t="s">
         <v>82</v>
       </c>
@@ -33649,51 +34007,51 @@
     </row>
     <row r="23" spans="1:37" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="40" t="s">
+      <c r="H24" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40" t="s">
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40" t="s">
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40" t="s">
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="U24" s="40"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="40" t="s">
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="X24" s="40"/>
-      <c r="Y24" s="40"/>
-      <c r="Z24" s="40" t="s">
+      <c r="X24" s="48"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="AA24" s="40"/>
-      <c r="AB24" s="40"/>
-      <c r="AC24" s="40" t="s">
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="48"/>
+      <c r="AC24" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="AD24" s="40"/>
-      <c r="AE24" s="40"/>
-      <c r="AF24" s="40" t="s">
+      <c r="AD24" s="48"/>
+      <c r="AE24" s="48"/>
+      <c r="AF24" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="AG24" s="40"/>
-      <c r="AH24" s="40"/>
+      <c r="AG24" s="48"/>
+      <c r="AH24" s="48"/>
     </row>
     <row r="25" spans="1:37" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H25" s="13" t="s">
@@ -34038,36 +34396,36 @@
     </row>
     <row r="35" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H36" s="40" t="s">
+      <c r="H36" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40" t="s">
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40" t="s">
+      <c r="L36" s="48"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="O36" s="40"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40" t="s">
+      <c r="O36" s="48"/>
+      <c r="P36" s="48"/>
+      <c r="Q36" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40" t="s">
+      <c r="R36" s="48"/>
+      <c r="S36" s="48"/>
+      <c r="T36" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="U36" s="40"/>
-      <c r="V36" s="40"/>
-      <c r="W36" s="40" t="s">
+      <c r="U36" s="48"/>
+      <c r="V36" s="48"/>
+      <c r="W36" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="X36" s="40"/>
-      <c r="Y36" s="40"/>
+      <c r="X36" s="48"/>
+      <c r="Y36" s="48"/>
     </row>
     <row r="37" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H37" s="13" t="s">
@@ -34348,16 +34706,16 @@
     </row>
     <row r="47" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H48" s="29" t="s">
+      <c r="H48" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29" t="s">
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
     </row>
     <row r="49" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H49" s="2" t="s">
@@ -34581,21 +34939,21 @@
     </row>
     <row r="59" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H60" s="40" t="s">
+      <c r="H60" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40" t="s">
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40" t="s">
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="O60" s="40"/>
-      <c r="P60" s="40"/>
+      <c r="O60" s="48"/>
+      <c r="P60" s="48"/>
     </row>
     <row r="61" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H61" s="2" t="s">
@@ -34834,21 +35192,21 @@
     </row>
     <row r="71" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="H72" s="29" t="s">
+      <c r="H72" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
-      <c r="K72" s="29" t="s">
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
+      <c r="K72" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="L72" s="29"/>
-      <c r="M72" s="29"/>
-      <c r="N72" s="29" t="s">
+      <c r="L72" s="47"/>
+      <c r="M72" s="47"/>
+      <c r="N72" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="O72" s="29"/>
-      <c r="P72" s="29"/>
+      <c r="O72" s="47"/>
+      <c r="P72" s="47"/>
     </row>
     <row r="73" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H73" s="2" t="s">
@@ -35106,7 +35464,7 @@
         <v>345594</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G81" t="s">
         <v>95</v>
       </c>
@@ -35150,7 +35508,7 @@
         <v>407790</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G82" t="s">
         <v>96</v>
       </c>
@@ -35179,30 +35537,30 @@
         <v>-62196</v>
       </c>
     </row>
-    <row r="83" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H84" s="29" t="s">
+    <row r="83" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H84" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="I84" s="29"/>
-      <c r="J84" s="29"/>
-      <c r="K84" s="29" t="s">
+      <c r="I84" s="47"/>
+      <c r="J84" s="47"/>
+      <c r="K84" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="L84" s="29"/>
-      <c r="M84" s="29"/>
-      <c r="N84" s="29" t="s">
+      <c r="L84" s="47"/>
+      <c r="M84" s="47"/>
+      <c r="N84" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="O84" s="29"/>
-      <c r="P84" s="29"/>
-      <c r="Q84" s="29" t="s">
+      <c r="O84" s="47"/>
+      <c r="P84" s="47"/>
+      <c r="Q84" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="R84" s="29"/>
-      <c r="S84" s="29"/>
-    </row>
-    <row r="85" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R84" s="47"/>
+      <c r="S84" s="47"/>
+    </row>
+    <row r="85" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H85" s="2" t="s">
         <v>40</v>
       </c>
@@ -35249,7 +35607,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -35266,7 +35624,7 @@
         <v>164057.1</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>189</v>
       </c>
@@ -35301,7 +35659,7 @@
         <v>56610</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>189</v>
       </c>
@@ -35324,7 +35682,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>233</v>
       </c>
@@ -35341,12 +35699,12 @@
         <v>98036.3</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G90" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G91" t="s">
         <v>9</v>
       </c>
@@ -35369,7 +35727,7 @@
         <v>219394</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G92" t="s">
         <v>36</v>
       </c>
@@ -35383,7 +35741,7 @@
         <v>19750</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>242</v>
       </c>
@@ -35464,12 +35822,8 @@
         <f>(J93+M93+P93+S93)</f>
         <v>519719</v>
       </c>
-      <c r="W93">
-        <f>(V93/U93)</f>
-        <v>7.4424189483331427</v>
-      </c>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
@@ -35486,9 +35840,85 @@
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
     </row>
-    <row r="95" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H96" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="I96" s="47"/>
+      <c r="J96" s="47"/>
+      <c r="K96" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="L96" s="47"/>
+      <c r="M96" s="47"/>
+    </row>
+    <row r="97" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H97" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M97" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B98">
+        <v>2427</v>
+      </c>
+      <c r="C98">
+        <v>11060</v>
+      </c>
+      <c r="D98">
+        <v>9841</v>
+      </c>
+      <c r="E98">
+        <v>71310.3</v>
+      </c>
+      <c r="H98">
+        <v>481</v>
+      </c>
+      <c r="K98">
+        <v>1940</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="37">
+    <mergeCell ref="H96:J96"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="Z24:AB24"/>
+    <mergeCell ref="AC24:AE24"/>
+    <mergeCell ref="AF24:AH24"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="T36:V36"/>
+    <mergeCell ref="W36:Y36"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
     <mergeCell ref="H84:J84"/>
     <mergeCell ref="K84:M84"/>
     <mergeCell ref="Q12:S12"/>
@@ -35505,25 +35935,6 @@
     <mergeCell ref="N60:P60"/>
     <mergeCell ref="N84:P84"/>
     <mergeCell ref="Q84:S84"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Z24:AB24"/>
-    <mergeCell ref="AC24:AE24"/>
-    <mergeCell ref="AF24:AH24"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="Q36:S36"/>
-    <mergeCell ref="T36:V36"/>
-    <mergeCell ref="W36:Y36"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35532,10 +35943,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617BFE3A-5538-4FC4-A07C-C660CA12141D}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35568,16 +35980,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>129</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>44393</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>245</v>
+      </c>
       <c r="B3" t="s">
         <v>137</v>
       </c>
@@ -35594,11 +36009,16 @@
         <v>138</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="J3" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>245</v>
+      </c>
       <c r="B4" t="s">
         <v>73</v>
       </c>
@@ -35619,6 +36039,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>245</v>
+      </c>
       <c r="B5" t="s">
         <v>130</v>
       </c>
@@ -35633,8 +36056,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>245</v>
+      </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C6">
         <v>1200</v>
@@ -35646,41 +36072,37 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H8" s="4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="C7" s="2">
+        <f>SUM(C3:C6)</f>
+        <v>4800</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(F3:F6)</f>
+        <v>9000</v>
+      </c>
+      <c r="I7" s="2">
+        <f>SUM(I4:I6)</f>
+        <v>28162</v>
+      </c>
+      <c r="J7" s="2">
+        <f>(C7+F7+I7)</f>
+        <v>41962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="4">
         <v>44400</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9">
-        <v>200</v>
-      </c>
-      <c r="E9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9">
-        <v>750</v>
-      </c>
-      <c r="H9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9">
-        <v>14260</v>
+      <c r="I9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -35688,22 +36110,22 @@
         <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C10">
         <v>200</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10">
         <v>750</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="I10">
-        <v>11723</v>
+        <v>14260</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -35711,16 +36133,22 @@
         <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="C11">
         <v>200</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="F11">
-        <v>1000</v>
+        <v>750</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11">
+        <v>11723</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -35728,7 +36156,7 @@
         <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="C12">
         <v>200</v>
@@ -35737,41 +36165,46 @@
         <v>45</v>
       </c>
       <c r="F12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13">
         <v>700</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>246</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="8">
         <v>950</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" t="s">
-        <v>252</v>
-      </c>
-      <c r="C15" s="8">
-        <v>200</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" t="s">
         <v>250</v>
-      </c>
-      <c r="B16" t="s">
-        <v>253</v>
       </c>
       <c r="C16" s="8">
         <v>200</v>
@@ -35779,7 +36212,15 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C17" s="2"/>
+      <c r="A17" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="8">
+        <v>200</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -35787,34 +36228,21 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19">
-        <v>250</v>
-      </c>
-      <c r="E19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19">
-        <v>750</v>
-      </c>
+      <c r="C19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>245</v>
+        <v>129</v>
       </c>
       <c r="C20">
         <v>250</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F20">
         <v>750</v>
@@ -35825,10 +36253,16 @@
         <v>189</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="C21">
         <v>250</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21">
+        <v>750</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -35836,7 +36270,7 @@
         <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>250</v>
@@ -35847,7 +36281,7 @@
         <v>189</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>130</v>
       </c>
       <c r="C23">
         <v>250</v>
@@ -35858,44 +36292,38 @@
         <v>189</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C24">
         <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" t="s">
+        <v>251</v>
+      </c>
+      <c r="C25">
+        <v>250</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26">
-        <v>200</v>
-      </c>
-      <c r="E26" t="s">
-        <v>132</v>
-      </c>
-      <c r="F26">
-        <v>750</v>
-      </c>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="C27">
         <v>200</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27">
         <v>750</v>
@@ -35906,10 +36334,16 @@
         <v>233</v>
       </c>
       <c r="B28" t="s">
-        <v>251</v>
+        <v>130</v>
       </c>
       <c r="C28">
         <v>200</v>
+      </c>
+      <c r="E28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28">
+        <v>750</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -35917,32 +36351,93 @@
         <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C29">
         <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C30" s="2">
-        <f>SUM(C9:C29)</f>
+      <c r="A30" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" t="s">
+        <v>251</v>
+      </c>
+      <c r="C30">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C31" s="2">
+        <f>SUM(C10:C30)</f>
         <v>4450</v>
       </c>
-      <c r="F30" s="2">
-        <f>SUM(F9:F29)</f>
+      <c r="F31" s="2">
+        <f>SUM(F10:F30)</f>
         <v>6200</v>
       </c>
-      <c r="I30" s="2">
-        <f>SUM(I9:I29)</f>
+      <c r="I31" s="2">
+        <f>SUM(I10:I30)</f>
         <v>25983</v>
       </c>
-      <c r="J30" s="2">
-        <f>(C30+F30+I30)</f>
+      <c r="J31" s="2">
+        <f>(C31+F31+I31)</f>
         <v>36633</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
+    <row r="32" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="29"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33">
+        <v>250</v>
+      </c>
+      <c r="E33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C36">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
26 temmuz hesapları işlendi
</commit_message>
<xml_diff>
--- a/Muhasebe.xlsx
+++ b/Muhasebe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BELEVİ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF11AA-2303-49F5-9C82-80D204606329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04D5035-F0A0-4E2E-B5C4-849DE436B28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="277">
   <si>
     <t>MÜSTAHSİL</t>
   </si>
@@ -813,9 +813,6 @@
     <t>HÜSEYİN ADSIZ</t>
   </si>
   <si>
-    <t>GÜLTEKİN EKİNCİ</t>
-  </si>
-  <si>
     <t>ŞABAN OK</t>
   </si>
   <si>
@@ -856,6 +853,27 @@
   </si>
   <si>
     <t>HAFTALIK TOPLAM</t>
+  </si>
+  <si>
+    <t>GÜLTEKİN ÖZDEMİR</t>
+  </si>
+  <si>
+    <t>26.7.2021/PAZARTESİ</t>
+  </si>
+  <si>
+    <t>Sıtkı Adsız</t>
+  </si>
+  <si>
+    <t>CEMAL ŞİMŞEK</t>
+  </si>
+  <si>
+    <t>BAHATTİN ADSIZ</t>
+  </si>
+  <si>
+    <t>SALİH ELDEN</t>
+  </si>
+  <si>
+    <t>27.7.2021/SALI</t>
   </si>
 </sst>
 </file>
@@ -1059,22 +1077,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1089,22 +1101,28 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1427,13 +1445,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BD046-FBF6-4454-99AD-0B843F600705}">
-  <dimension ref="A1:BQ419"/>
+  <dimension ref="A1:BQ435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B395" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B421" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BP418" sqref="BP418"/>
+      <selection pane="bottomRight" activeCell="J439" sqref="J439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1503,90 +1521,90 @@
         <v>171</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="35" t="s">
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="33" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="36" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="40" t="s">
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="36" t="s">
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="39" t="s">
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="38" t="s">
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="35" t="s">
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="AS1" s="35"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="35"/>
-      <c r="AV1" s="34" t="s">
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="33" t="s">
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="37" t="s">
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="37"/>
-      <c r="BG1" s="37"/>
-      <c r="BH1" s="31" t="s">
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="35"/>
+      <c r="BH1" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="32" t="s">
+      <c r="BI1" s="39"/>
+      <c r="BJ1" s="39"/>
+      <c r="BK1" s="39"/>
+      <c r="BL1" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="32"/>
-      <c r="BO1" s="32"/>
+      <c r="BM1" s="40"/>
+      <c r="BN1" s="40"/>
+      <c r="BO1" s="40"/>
       <c r="BP1" s="2" t="s">
         <v>82</v>
       </c>
@@ -32548,10 +32566,10 @@
     </row>
     <row r="411" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A411" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B411" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D411">
         <v>486</v>
@@ -32582,10 +32600,10 @@
     </row>
     <row r="412" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A412" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B412" t="s">
         <v>265</v>
-      </c>
-      <c r="B412" t="s">
-        <v>266</v>
       </c>
       <c r="D412">
         <v>48</v>
@@ -32610,7 +32628,7 @@
     </row>
     <row r="413" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A413" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B413" t="s">
         <v>14</v>
@@ -32638,10 +32656,10 @@
     </row>
     <row r="414" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A414" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B414" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D414">
         <v>759</v>
@@ -32666,7 +32684,7 @@
     </row>
     <row r="415" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A415" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B415" t="s">
         <v>124</v>
@@ -32694,7 +32712,7 @@
     </row>
     <row r="416" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A416" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B416" t="s">
         <v>124</v>
@@ -32722,7 +32740,7 @@
     </row>
     <row r="417" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A417" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B417" t="s">
         <v>8</v>
@@ -32793,8 +32811,463 @@
         <v>7.1128571428571421</v>
       </c>
     </row>
+    <row r="420" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A420" s="10"/>
+    </row>
+    <row r="422" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A422" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B422" t="s">
+        <v>149</v>
+      </c>
+      <c r="C422" t="s">
+        <v>9</v>
+      </c>
+      <c r="D422">
+        <v>430</v>
+      </c>
+      <c r="E422">
+        <v>1520</v>
+      </c>
+      <c r="F422">
+        <v>180</v>
+      </c>
+      <c r="G422">
+        <f t="shared" ref="G422:G433" si="92">(E422-F422)</f>
+        <v>1340</v>
+      </c>
+      <c r="H422">
+        <v>6.71</v>
+      </c>
+      <c r="I422">
+        <f t="shared" ref="I422:I433" si="93">(G422*H422)</f>
+        <v>8991.4</v>
+      </c>
+      <c r="BD422">
+        <v>578</v>
+      </c>
+      <c r="BF422" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH422">
+        <v>2784</v>
+      </c>
+      <c r="BJ422" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="423" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A423" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B423" t="s">
+        <v>28</v>
+      </c>
+      <c r="C423" t="s">
+        <v>9</v>
+      </c>
+      <c r="D423">
+        <v>1062</v>
+      </c>
+      <c r="E423">
+        <v>4280</v>
+      </c>
+      <c r="F423">
+        <v>430</v>
+      </c>
+      <c r="G423">
+        <f t="shared" si="92"/>
+        <v>3850</v>
+      </c>
+      <c r="H423">
+        <v>7.3</v>
+      </c>
+      <c r="I423">
+        <f t="shared" si="93"/>
+        <v>28105</v>
+      </c>
+      <c r="BD423">
+        <v>1048</v>
+      </c>
+      <c r="BF423" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH423">
+        <v>288</v>
+      </c>
+      <c r="BJ423" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="424" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A424" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B424" t="s">
+        <v>8</v>
+      </c>
+      <c r="C424" t="s">
+        <v>9</v>
+      </c>
+      <c r="D424">
+        <v>40</v>
+      </c>
+      <c r="E424">
+        <v>140</v>
+      </c>
+      <c r="F424">
+        <v>20</v>
+      </c>
+      <c r="G424">
+        <f t="shared" si="92"/>
+        <v>120</v>
+      </c>
+      <c r="H424">
+        <v>4</v>
+      </c>
+      <c r="I424">
+        <f t="shared" si="93"/>
+        <v>480</v>
+      </c>
+      <c r="BH424" s="2"/>
+    </row>
+    <row r="425" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A425" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B425" t="s">
+        <v>26</v>
+      </c>
+      <c r="C425" t="s">
+        <v>9</v>
+      </c>
+      <c r="D425">
+        <v>345</v>
+      </c>
+      <c r="E425">
+        <v>2220</v>
+      </c>
+      <c r="F425">
+        <v>320</v>
+      </c>
+      <c r="G425">
+        <f t="shared" si="92"/>
+        <v>1900</v>
+      </c>
+      <c r="H425">
+        <v>7.36</v>
+      </c>
+      <c r="I425">
+        <f t="shared" si="93"/>
+        <v>13984</v>
+      </c>
+    </row>
+    <row r="426" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A426" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B426" t="s">
+        <v>124</v>
+      </c>
+      <c r="C426" t="s">
+        <v>9</v>
+      </c>
+      <c r="D426">
+        <v>114</v>
+      </c>
+      <c r="E426">
+        <v>440</v>
+      </c>
+      <c r="F426">
+        <v>50</v>
+      </c>
+      <c r="G426">
+        <f t="shared" si="92"/>
+        <v>390</v>
+      </c>
+      <c r="H426">
+        <v>5</v>
+      </c>
+      <c r="I426">
+        <f t="shared" si="93"/>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="427" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A427" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B427" t="s">
+        <v>229</v>
+      </c>
+      <c r="C427" t="s">
+        <v>36</v>
+      </c>
+      <c r="D427">
+        <v>640</v>
+      </c>
+      <c r="E427">
+        <v>2680</v>
+      </c>
+      <c r="F427">
+        <v>256</v>
+      </c>
+      <c r="G427">
+        <f t="shared" si="92"/>
+        <v>2424</v>
+      </c>
+      <c r="H427">
+        <v>8.83</v>
+      </c>
+      <c r="I427">
+        <f t="shared" si="93"/>
+        <v>21403.920000000002</v>
+      </c>
+    </row>
+    <row r="428" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A428" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B428" t="s">
+        <v>272</v>
+      </c>
+      <c r="C428" t="s">
+        <v>9</v>
+      </c>
+      <c r="D428">
+        <v>440</v>
+      </c>
+      <c r="E428">
+        <v>1620</v>
+      </c>
+      <c r="F428">
+        <v>220</v>
+      </c>
+      <c r="G428">
+        <f t="shared" si="92"/>
+        <v>1400</v>
+      </c>
+      <c r="H428">
+        <v>6.75</v>
+      </c>
+      <c r="I428">
+        <f t="shared" si="93"/>
+        <v>9450</v>
+      </c>
+    </row>
+    <row r="429" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A429" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B429" t="s">
+        <v>266</v>
+      </c>
+      <c r="C429" t="s">
+        <v>9</v>
+      </c>
+      <c r="D429">
+        <v>722</v>
+      </c>
+      <c r="E429">
+        <v>2980</v>
+      </c>
+      <c r="F429">
+        <v>290</v>
+      </c>
+      <c r="G429">
+        <f t="shared" si="92"/>
+        <v>2690</v>
+      </c>
+      <c r="H429">
+        <v>7.35</v>
+      </c>
+      <c r="I429">
+        <f t="shared" si="93"/>
+        <v>19771.5</v>
+      </c>
+    </row>
+    <row r="430" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A430" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B430" t="s">
+        <v>14</v>
+      </c>
+      <c r="C430" t="s">
+        <v>9</v>
+      </c>
+      <c r="D430">
+        <v>112</v>
+      </c>
+      <c r="E430">
+        <v>600</v>
+      </c>
+      <c r="F430">
+        <v>112</v>
+      </c>
+      <c r="G430">
+        <f t="shared" si="92"/>
+        <v>488</v>
+      </c>
+      <c r="H430">
+        <v>6.75</v>
+      </c>
+      <c r="I430">
+        <f t="shared" si="93"/>
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="431" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A431" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B431" t="s">
+        <v>22</v>
+      </c>
+      <c r="C431" t="s">
+        <v>9</v>
+      </c>
+      <c r="D431">
+        <v>57</v>
+      </c>
+      <c r="E431">
+        <v>240</v>
+      </c>
+      <c r="F431">
+        <v>30</v>
+      </c>
+      <c r="G431">
+        <f t="shared" si="92"/>
+        <v>210</v>
+      </c>
+      <c r="H431">
+        <v>5</v>
+      </c>
+      <c r="I431">
+        <f t="shared" si="93"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="432" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A432" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B432" t="s">
+        <v>15</v>
+      </c>
+      <c r="C432" t="s">
+        <v>9</v>
+      </c>
+      <c r="D432">
+        <v>510</v>
+      </c>
+      <c r="E432">
+        <v>2522</v>
+      </c>
+      <c r="F432">
+        <v>204</v>
+      </c>
+      <c r="G432">
+        <f t="shared" si="92"/>
+        <v>2318</v>
+      </c>
+      <c r="H432">
+        <v>7.5</v>
+      </c>
+      <c r="I432">
+        <f t="shared" si="93"/>
+        <v>17385</v>
+      </c>
+    </row>
+    <row r="433" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A433" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B433" t="s">
+        <v>15</v>
+      </c>
+      <c r="C433" t="s">
+        <v>36</v>
+      </c>
+      <c r="D433">
+        <v>226</v>
+      </c>
+      <c r="E433">
+        <v>1117</v>
+      </c>
+      <c r="F433">
+        <v>90</v>
+      </c>
+      <c r="G433">
+        <f t="shared" si="92"/>
+        <v>1027</v>
+      </c>
+      <c r="H433">
+        <v>9</v>
+      </c>
+      <c r="I433">
+        <f t="shared" si="93"/>
+        <v>9243</v>
+      </c>
+    </row>
+    <row r="434" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A434" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B434" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D434" s="2">
+        <f t="shared" ref="D434:I434" si="94">SUM(D422:D433)</f>
+        <v>4698</v>
+      </c>
+      <c r="E434" s="2">
+        <f t="shared" si="94"/>
+        <v>20359</v>
+      </c>
+      <c r="F434" s="2">
+        <f t="shared" si="94"/>
+        <v>2202</v>
+      </c>
+      <c r="G434" s="2">
+        <f t="shared" si="94"/>
+        <v>18157</v>
+      </c>
+      <c r="H434" s="2"/>
+      <c r="I434" s="2">
+        <f t="shared" si="94"/>
+        <v>135107.82</v>
+      </c>
+      <c r="BD434" s="2">
+        <f>SUM(BD422:BD433)</f>
+        <v>1626</v>
+      </c>
+      <c r="BH434" s="2">
+        <f>SUM(BH422:BH433)</f>
+        <v>3072</v>
+      </c>
+      <c r="BP434">
+        <f>(BD434+BH434)</f>
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="435" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="B435" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H435" s="2">
+        <f>AVERAGE(H422:H433)</f>
+        <v>6.7958333333333334</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="BH1:BK1"/>
+    <mergeCell ref="BL1:BO1"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="X1:AA1"/>
@@ -32804,11 +33277,6 @@
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="BH1:BK1"/>
-    <mergeCell ref="BL1:BO1"/>
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AR1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32891,10 +33359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD1A8C-99DF-4166-8097-144C71FF7489}">
-  <dimension ref="A1:BQ6"/>
+  <dimension ref="A1:CF8"/>
   <sheetViews>
-    <sheetView topLeftCell="BH1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView topLeftCell="AE1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32905,112 +33373,134 @@
     <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="5.90625" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="28"/>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
       <c r="O1" s="27"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="U1" s="40" t="s">
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="U1" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Z1" s="32" t="s">
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Z1" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AE1" s="44" t="s">
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AE1" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AJ1" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AJ1" s="37" t="s">
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AO1" s="44" t="s">
         <v>257</v>
       </c>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AO1" s="45" t="s">
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AT1" s="41" t="s">
         <v>258</v>
       </c>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
-      <c r="AR1" s="45"/>
-      <c r="AT1" s="46" t="s">
+      <c r="AU1" s="41"/>
+      <c r="AV1" s="41"/>
+      <c r="AW1" s="41"/>
+      <c r="AY1" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AY1" s="42" t="s">
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="46"/>
+      <c r="BB1" s="46"/>
+      <c r="BD1" s="43" t="s">
         <v>260</v>
-      </c>
-      <c r="AZ1" s="42"/>
-      <c r="BA1" s="42"/>
-      <c r="BB1" s="42"/>
-      <c r="BD1" s="43" t="s">
-        <v>261</v>
       </c>
       <c r="BE1" s="43"/>
       <c r="BF1" s="43"/>
       <c r="BG1" s="43"/>
-      <c r="BI1" s="34" t="s">
+      <c r="BI1" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BN1" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="BJ1" s="34"/>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BN1" s="35" t="s">
-        <v>269</v>
-      </c>
-      <c r="BO1" s="35"/>
-      <c r="BP1" s="35"/>
-      <c r="BQ1" s="35"/>
-    </row>
-    <row r="2" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BS1" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="BT1" s="41"/>
+      <c r="BU1" s="41"/>
+      <c r="BV1" s="41"/>
+      <c r="BX1" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="BY1" s="42"/>
+      <c r="BZ1" s="42"/>
+      <c r="CA1" s="42"/>
+      <c r="CC1" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="CD1" s="43"/>
+      <c r="CE1" s="43"/>
+      <c r="CF1" s="43"/>
+    </row>
+    <row r="2" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>234</v>
@@ -33019,10 +33509,10 @@
         <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>234</v>
@@ -33031,10 +33521,10 @@
         <v>59</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>234</v>
@@ -33043,10 +33533,10 @@
         <v>59</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>234</v>
@@ -33055,10 +33545,10 @@
         <v>59</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>234</v>
@@ -33067,10 +33557,10 @@
         <v>59</v>
       </c>
       <c r="AA2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>234</v>
@@ -33079,10 +33569,10 @@
         <v>59</v>
       </c>
       <c r="AF2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>234</v>
@@ -33091,10 +33581,10 @@
         <v>59</v>
       </c>
       <c r="AK2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="AM2" s="2" t="s">
         <v>234</v>
@@ -33103,10 +33593,10 @@
         <v>59</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>234</v>
@@ -33115,10 +33605,10 @@
         <v>59</v>
       </c>
       <c r="AU2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>234</v>
@@ -33127,10 +33617,10 @@
         <v>59</v>
       </c>
       <c r="AZ2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BA2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="BB2" s="2" t="s">
         <v>234</v>
@@ -33139,10 +33629,10 @@
         <v>59</v>
       </c>
       <c r="BE2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BF2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="BG2" s="2" t="s">
         <v>234</v>
@@ -33151,10 +33641,10 @@
         <v>59</v>
       </c>
       <c r="BJ2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BK2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="BL2" s="2" t="s">
         <v>234</v>
@@ -33163,16 +33653,52 @@
         <v>59</v>
       </c>
       <c r="BO2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="BP2" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="BQ2" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BS2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>38000</v>
       </c>
@@ -33317,8 +33843,38 @@
         <f>(BO3-BP3)</f>
         <v>21925</v>
       </c>
-    </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BS3" s="1">
+        <v>44403</v>
+      </c>
+      <c r="BT3">
+        <v>1050</v>
+      </c>
+      <c r="BV3">
+        <f>(BT3-BU3)</f>
+        <v>1050</v>
+      </c>
+      <c r="BX3" s="1">
+        <v>44403</v>
+      </c>
+      <c r="BY3">
+        <v>21396</v>
+      </c>
+      <c r="CA3">
+        <f>(BY3-BZ3)</f>
+        <v>21396</v>
+      </c>
+      <c r="CC3" s="1">
+        <v>44403</v>
+      </c>
+      <c r="CD3">
+        <v>9000</v>
+      </c>
+      <c r="CF3">
+        <f>(CD3-CE3)</f>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44402</v>
       </c>
@@ -33352,6 +33908,16 @@
         <f>(L4-M4+N3)</f>
         <v>34758</v>
       </c>
+      <c r="AJ4" s="1">
+        <v>44403</v>
+      </c>
+      <c r="AK4">
+        <v>26628</v>
+      </c>
+      <c r="AM4">
+        <f>(AK4-AL4+AM3)</f>
+        <v>55575</v>
+      </c>
       <c r="AV4">
         <v>10000</v>
       </c>
@@ -33360,8 +33926,31 @@
         <v>15737</v>
       </c>
       <c r="AY4" s="1"/>
-    </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BN4" s="1">
+        <v>44403</v>
+      </c>
+      <c r="BO4">
+        <v>19775</v>
+      </c>
+      <c r="BP4">
+        <v>18500</v>
+      </c>
+      <c r="BQ4">
+        <f>(BO4-BP4+BQ3)</f>
+        <v>23200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44403</v>
+      </c>
+      <c r="B5">
+        <v>480</v>
+      </c>
+      <c r="D5">
+        <f>(B5-C5+D4)</f>
+        <v>20880</v>
+      </c>
       <c r="F5" s="1">
         <v>44400</v>
       </c>
@@ -33386,8 +33975,18 @@
         <v>41758</v>
       </c>
       <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="AT5" s="1">
+        <v>44403</v>
+      </c>
+      <c r="AU5">
+        <v>28100</v>
+      </c>
+      <c r="AW5">
+        <f>(AW4+AU5-AV5)</f>
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:84" x14ac:dyDescent="0.35">
       <c r="F6" s="1">
         <v>44402</v>
       </c>
@@ -33412,8 +34011,49 @@
         <v>31093</v>
       </c>
     </row>
+    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="F7" s="1">
+        <v>44403</v>
+      </c>
+      <c r="G7">
+        <v>3290</v>
+      </c>
+      <c r="H7">
+        <v>1400</v>
+      </c>
+      <c r="I7">
+        <f>(G7-H7+I6)</f>
+        <v>89682</v>
+      </c>
+      <c r="K7" s="1">
+        <v>44403</v>
+      </c>
+      <c r="L7">
+        <v>14000</v>
+      </c>
+      <c r="N7">
+        <f>(L7-M7+N6)</f>
+        <v>45093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="K8" s="1">
+        <v>44403</v>
+      </c>
+      <c r="L8">
+        <v>1950</v>
+      </c>
+      <c r="N8">
+        <f>(L8-M8+N7)</f>
+        <v>47043</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="BS1:BV1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CF1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="U1:X1"/>
@@ -33427,7 +34067,6 @@
     <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BD1:BG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33435,10 +34074,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F781AA57-6247-4A4F-9752-70CC607DC978}">
-  <dimension ref="A1:AK98"/>
+  <dimension ref="A1:AK99"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView topLeftCell="A67" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35875,7 +36514,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B98">
         <v>2427</v>
@@ -35896,8 +36535,52 @@
         <v>1940</v>
       </c>
     </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>271</v>
+      </c>
+      <c r="B99">
+        <v>4698</v>
+      </c>
+      <c r="C99">
+        <v>20359</v>
+      </c>
+      <c r="D99">
+        <v>18157</v>
+      </c>
+      <c r="E99">
+        <v>135107.79999999999</v>
+      </c>
+      <c r="H99">
+        <v>1626</v>
+      </c>
+      <c r="K99">
+        <v>6144</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="H84:J84"/>
+    <mergeCell ref="K84:M84"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="N72:P72"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="Q84:S84"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
     <mergeCell ref="H96:J96"/>
     <mergeCell ref="K96:M96"/>
     <mergeCell ref="Z24:AB24"/>
@@ -35914,27 +36597,6 @@
     <mergeCell ref="N24:P24"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="T24:V24"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="H84:J84"/>
-    <mergeCell ref="K84:M84"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="N72:P72"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="Q84:S84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35943,11 +36605,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617BFE3A-5538-4FC4-A07C-C660CA12141D}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36012,7 +36674,7 @@
         <v>247</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -36391,7 +37053,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
         <v>73</v>
@@ -36408,7 +37070,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -36419,7 +37081,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B35" t="s">
         <v>249</v>
@@ -36430,13 +37092,74 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B36" t="s">
         <v>251</v>
       </c>
       <c r="C36">
         <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38">
+        <v>250</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39">
+        <v>250</v>
+      </c>
+      <c r="E39" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" t="s">
+        <v>249</v>
+      </c>
+      <c r="C40">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" t="s">
+        <v>251</v>
+      </c>
+      <c r="C41">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -36450,7 +37173,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
31 temmuz 3 kişiye ödeme yapıldı
</commit_message>
<xml_diff>
--- a/Muhasebe.xlsx
+++ b/Muhasebe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BELEVİ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A943CEE-0781-4B7D-9983-D46A1F620777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439F91A-2725-4F85-9668-DE9B2CF1EBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" activeTab="2" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
   </bookViews>
@@ -1213,22 +1213,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1243,13 +1237,10 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1258,7 +1249,16 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1584,7 +1584,7 @@
   <dimension ref="A1:BQ502"/>
   <sheetViews>
     <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B493" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B491" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="M492" sqref="M492"/>
@@ -1657,90 +1657,90 @@
         <v>159</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="40" t="s">
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="38" t="s">
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="41" t="s">
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="45" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="41" t="s">
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="AG1" s="41"/>
-      <c r="AH1" s="41"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="44" t="s">
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="43" t="s">
+      <c r="AK1" s="42"/>
+      <c r="AL1" s="42"/>
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AQ1" s="43"/>
-      <c r="AR1" s="40" t="s">
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="39" t="s">
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="AW1" s="39"/>
-      <c r="AX1" s="39"/>
-      <c r="AY1" s="39"/>
-      <c r="AZ1" s="38" t="s">
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="38"/>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="42" t="s">
+      <c r="BA1" s="39"/>
+      <c r="BB1" s="39"/>
+      <c r="BC1" s="39"/>
+      <c r="BD1" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="42"/>
-      <c r="BF1" s="42"/>
-      <c r="BG1" s="42"/>
-      <c r="BH1" s="36" t="s">
+      <c r="BE1" s="40"/>
+      <c r="BF1" s="40"/>
+      <c r="BG1" s="40"/>
+      <c r="BH1" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="36"/>
-      <c r="BJ1" s="36"/>
-      <c r="BK1" s="36"/>
-      <c r="BL1" s="37" t="s">
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
+      <c r="BL1" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="37"/>
-      <c r="BN1" s="37"/>
-      <c r="BO1" s="37"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="45"/>
       <c r="BP1" s="2" t="s">
         <v>82</v>
       </c>
@@ -36672,6 +36672,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="BH1:BK1"/>
+    <mergeCell ref="BL1:BO1"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="X1:AA1"/>
@@ -36681,11 +36686,6 @@
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="BH1:BK1"/>
-    <mergeCell ref="BL1:BO1"/>
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AR1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44173,8 +44173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD1A8C-99DF-4166-8097-144C71FF7489}">
   <dimension ref="A1:BV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44197,99 +44197,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
       <c r="E1" s="26"/>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="27"/>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
       <c r="O1" s="25"/>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="U1" s="45" t="s">
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="U1" s="43" t="s">
         <v>299</v>
       </c>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Z1" s="37" t="s">
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Z1" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AE1" s="42" t="s">
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AE1" s="40" t="s">
         <v>239</v>
       </c>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AJ1" s="48" t="s">
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AJ1" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AO1" s="47" t="s">
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AO1" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AT1" s="50" t="s">
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AT1" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="AU1" s="50"/>
-      <c r="AV1" s="50"/>
-      <c r="AW1" s="50"/>
-      <c r="AY1" s="39" t="s">
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
+      <c r="AW1" s="47"/>
+      <c r="AY1" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="AZ1" s="39"/>
-      <c r="BA1" s="39"/>
-      <c r="BB1" s="39"/>
-      <c r="BD1" s="47" t="s">
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BD1" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="BE1" s="47"/>
-      <c r="BF1" s="47"/>
-      <c r="BG1" s="47"/>
-      <c r="BI1" s="46" t="s">
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BI1" s="49" t="s">
         <v>300</v>
       </c>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BN1" s="51" t="s">
+      <c r="BJ1" s="49"/>
+      <c r="BK1" s="49"/>
+      <c r="BL1" s="49"/>
+      <c r="BN1" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="BO1" s="51"/>
-      <c r="BP1" s="51"/>
-      <c r="BQ1" s="51"/>
-      <c r="BS1" s="49" t="s">
+      <c r="BO1" s="50"/>
+      <c r="BP1" s="50"/>
+      <c r="BQ1" s="50"/>
+      <c r="BS1" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="49"/>
-      <c r="BV1" s="49"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
     </row>
     <row r="2" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -44673,6 +44673,16 @@
         <f>(Q4-R4+S3)</f>
         <v>37000</v>
       </c>
+      <c r="U4" s="1">
+        <v>44408</v>
+      </c>
+      <c r="W4">
+        <v>10000</v>
+      </c>
+      <c r="X4">
+        <f>(V4-W4+X3)</f>
+        <v>10300</v>
+      </c>
       <c r="AE4" s="1">
         <v>44403</v>
       </c>
@@ -44797,6 +44807,26 @@
       <c r="AR5">
         <f>(AR4+AP5-AQ5)</f>
         <v>43837</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>44408</v>
+      </c>
+      <c r="AV5">
+        <v>10000</v>
+      </c>
+      <c r="AW5">
+        <f>(AU5-AV5+AW4)</f>
+        <v>7185</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>44408</v>
+      </c>
+      <c r="BF5">
+        <v>5000</v>
+      </c>
+      <c r="BG5">
+        <f>(BE5-BF5+BG4)</f>
+        <v>7000</v>
       </c>
     </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.35">
@@ -44982,12 +45012,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="BS1:BV1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="BD1:BG1"/>
-    <mergeCell ref="BI1:BL1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="AY1:BB1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="U1:X1"/>
@@ -44997,6 +45021,12 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="P1:S1"/>
+    <mergeCell ref="BS1:BV1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="BI1:BL1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="AY1:BB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47527,6 +47557,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="H84:J84"/>
+    <mergeCell ref="K84:M84"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="N72:P72"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="Q84:S84"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
     <mergeCell ref="H96:J96"/>
     <mergeCell ref="K96:M96"/>
     <mergeCell ref="Z24:AB24"/>
@@ -47543,27 +47594,6 @@
     <mergeCell ref="N24:P24"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="T24:V24"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="H84:J84"/>
-    <mergeCell ref="K84:M84"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="N72:P72"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="Q84:S84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ağustos ayına giriş yapıldı
</commit_message>
<xml_diff>
--- a/Muhasebe.xlsx
+++ b/Muhasebe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BELEVİ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439F91A-2725-4F85-9668-DE9B2CF1EBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132FC769-E470-4A65-9F9A-016E006D77D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" activeTab="2" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GÜNLÜK_GELEN_GİDEN_MAL" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="321">
   <si>
     <t>MÜSTAHSİL</t>
   </si>
@@ -855,9 +855,6 @@
     <t>35 LEC 21</t>
   </si>
   <si>
-    <t>9 TL FARKLI</t>
-  </si>
-  <si>
     <t>35 AUD 236</t>
   </si>
   <si>
@@ -1010,6 +1007,9 @@
   <si>
     <t xml:space="preserve">BAYRAM ADSIZ </t>
   </si>
+  <si>
+    <t>1.8.2021/PAZAR</t>
+  </si>
 </sst>
 </file>
 
@@ -1156,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1213,16 +1213,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1237,10 +1246,13 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1249,16 +1261,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1581,13 +1584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BD046-FBF6-4454-99AD-0B843F600705}">
-  <dimension ref="A1:BQ502"/>
+  <dimension ref="A1:BQ506"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B491" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B488" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M492" sqref="M492"/>
+      <selection pane="bottomRight" activeCell="A506" sqref="A506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1657,90 +1660,90 @@
         <v>159</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="36" t="s">
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
       <c r="T1" s="39" t="s">
         <v>213</v>
       </c>
       <c r="U1" s="39"/>
       <c r="V1" s="39"/>
       <c r="W1" s="39"/>
-      <c r="X1" s="38" t="s">
+      <c r="X1" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="43" t="s">
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="38" t="s">
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="42" t="s">
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="AK1" s="42"/>
-      <c r="AL1" s="42"/>
-      <c r="AM1" s="42"/>
-      <c r="AN1" s="41" t="s">
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="AO1" s="41"/>
-      <c r="AP1" s="41"/>
-      <c r="AQ1" s="41"/>
-      <c r="AR1" s="36" t="s">
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="AS1" s="36"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="36"/>
-      <c r="AV1" s="37" t="s">
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
+      <c r="AU1" s="41"/>
+      <c r="AV1" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="AW1" s="37"/>
-      <c r="AX1" s="37"/>
-      <c r="AY1" s="37"/>
+      <c r="AW1" s="40"/>
+      <c r="AX1" s="40"/>
+      <c r="AY1" s="40"/>
       <c r="AZ1" s="39" t="s">
         <v>203</v>
       </c>
       <c r="BA1" s="39"/>
       <c r="BB1" s="39"/>
       <c r="BC1" s="39"/>
-      <c r="BD1" s="40" t="s">
+      <c r="BD1" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="BE1" s="40"/>
-      <c r="BF1" s="40"/>
-      <c r="BG1" s="40"/>
-      <c r="BH1" s="44" t="s">
+      <c r="BE1" s="43"/>
+      <c r="BF1" s="43"/>
+      <c r="BG1" s="43"/>
+      <c r="BH1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="45" t="s">
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="37"/>
+      <c r="BK1" s="37"/>
+      <c r="BL1" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="45"/>
-      <c r="BN1" s="45"/>
-      <c r="BO1" s="45"/>
+      <c r="BM1" s="38"/>
+      <c r="BN1" s="38"/>
+      <c r="BO1" s="38"/>
       <c r="BP1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I5">
         <v>3500.85</v>
@@ -2570,7 +2573,7 @@
         <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I11">
         <v>3014.4</v>
@@ -3196,7 +3199,7 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I19">
         <v>3909.75</v>
@@ -4027,7 +4030,7 @@
         <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4327,7 +4330,7 @@
       <c r="BO32" s="11"/>
       <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>134</v>
       </c>
@@ -4417,7 +4420,7 @@
       <c r="BO33" s="11"/>
       <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>134</v>
       </c>
@@ -4507,7 +4510,7 @@
       <c r="BO34" s="11"/>
       <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>134</v>
       </c>
@@ -4597,12 +4600,12 @@
       <c r="BO35" s="11"/>
       <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -4673,7 +4676,7 @@
       <c r="BO36" s="29"/>
       <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>17</v>
       </c>
@@ -4759,7 +4762,7 @@
       <c r="BO37" s="11"/>
       <c r="BP37" s="2"/>
     </row>
-    <row r="38" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>18</v>
       </c>
@@ -4833,78 +4836,77 @@
       <c r="BO38" s="11"/>
       <c r="BP38" s="2"/>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
-      <c r="W39" s="10"/>
-      <c r="X39" s="10"/>
-      <c r="Y39" s="10"/>
-      <c r="Z39" s="10"/>
-      <c r="AA39" s="10"/>
-      <c r="AB39" s="10"/>
-      <c r="AC39" s="10"/>
-      <c r="AD39" s="10"/>
-      <c r="AE39" s="10"/>
-      <c r="AF39" s="10"/>
-      <c r="AG39" s="10"/>
-      <c r="AH39" s="10"/>
-      <c r="AI39" s="10"/>
-      <c r="AJ39" s="10"/>
-      <c r="AK39" s="10"/>
-      <c r="AL39" s="10"/>
-      <c r="AM39" s="10"/>
-      <c r="AN39" s="10"/>
-      <c r="AO39" s="10"/>
-      <c r="AP39" s="10"/>
-      <c r="AQ39" s="10"/>
-      <c r="AR39" s="10"/>
-      <c r="AS39" s="10"/>
-      <c r="AT39" s="10"/>
-      <c r="AU39" s="10"/>
-      <c r="AV39" s="10"/>
-      <c r="AW39" s="10"/>
-      <c r="AX39" s="10"/>
-      <c r="AY39" s="10"/>
-      <c r="AZ39" s="10"/>
-      <c r="BA39" s="10"/>
-      <c r="BB39" s="10"/>
-      <c r="BC39" s="10"/>
-      <c r="BD39" s="18"/>
-      <c r="BE39" s="18"/>
-      <c r="BF39" s="18"/>
-      <c r="BG39" s="18"/>
-      <c r="BH39" s="18"/>
-      <c r="BI39" s="18"/>
-      <c r="BJ39" s="18"/>
-      <c r="BK39" s="18"/>
-      <c r="BL39" s="18"/>
-      <c r="BM39" s="18"/>
-      <c r="BN39" s="18"/>
-      <c r="BO39" s="18"/>
-      <c r="BP39" s="10"/>
-      <c r="BQ39" s="9"/>
-    </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:68" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="31"/>
+      <c r="AH39" s="31"/>
+      <c r="AI39" s="31"/>
+      <c r="AJ39" s="31"/>
+      <c r="AK39" s="31"/>
+      <c r="AL39" s="31"/>
+      <c r="AM39" s="31"/>
+      <c r="AN39" s="31"/>
+      <c r="AO39" s="31"/>
+      <c r="AP39" s="31"/>
+      <c r="AQ39" s="31"/>
+      <c r="AR39" s="31"/>
+      <c r="AS39" s="31"/>
+      <c r="AT39" s="31"/>
+      <c r="AU39" s="31"/>
+      <c r="AV39" s="31"/>
+      <c r="AW39" s="31"/>
+      <c r="AX39" s="31"/>
+      <c r="AY39" s="31"/>
+      <c r="AZ39" s="31"/>
+      <c r="BA39" s="31"/>
+      <c r="BB39" s="31"/>
+      <c r="BC39" s="31"/>
+      <c r="BD39" s="36"/>
+      <c r="BE39" s="36"/>
+      <c r="BF39" s="36"/>
+      <c r="BG39" s="36"/>
+      <c r="BH39" s="36"/>
+      <c r="BI39" s="36"/>
+      <c r="BJ39" s="36"/>
+      <c r="BK39" s="36"/>
+      <c r="BL39" s="36"/>
+      <c r="BM39" s="36"/>
+      <c r="BN39" s="36"/>
+      <c r="BO39" s="36"/>
+      <c r="BP39" s="31"/>
+    </row>
+    <row r="40" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B40" s="17"/>
       <c r="C40" s="8" t="s">
         <v>9</v>
@@ -4993,7 +4995,7 @@
       <c r="BO40" s="11"/>
       <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>138</v>
       </c>
@@ -5083,7 +5085,7 @@
       <c r="BO41" s="11"/>
       <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>138</v>
       </c>
@@ -5173,7 +5175,7 @@
       <c r="BO42" s="11"/>
       <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>138</v>
       </c>
@@ -5263,7 +5265,7 @@
       <c r="BO43" s="11"/>
       <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>138</v>
       </c>
@@ -5353,7 +5355,7 @@
       <c r="BO44" s="11"/>
       <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>138</v>
       </c>
@@ -5443,7 +5445,7 @@
       <c r="BO45" s="11"/>
       <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>138</v>
       </c>
@@ -5533,7 +5535,7 @@
       <c r="BO46" s="11"/>
       <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -5623,12 +5625,12 @@
       <c r="BO47" s="11"/>
       <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -6586,7 +6588,7 @@
         <v>142</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -7556,7 +7558,7 @@
         <v>145</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -8787,7 +8789,7 @@
         <v>149</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -9847,7 +9849,7 @@
         <v>153</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
@@ -9918,7 +9920,7 @@
       <c r="BO96" s="29"/>
       <c r="BP96" s="2"/>
     </row>
-    <row r="97" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B97" s="2" t="s">
         <v>17</v>
       </c>
@@ -10016,7 +10018,7 @@
         <v>4793</v>
       </c>
     </row>
-    <row r="98" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B98" s="2" t="s">
         <v>18</v>
       </c>
@@ -10090,7 +10092,7 @@
       <c r="BO98" s="11"/>
       <c r="BP98" s="2"/>
     </row>
-    <row r="99" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -10159,7 +10161,7 @@
       <c r="BO99" s="11"/>
       <c r="BP99" s="2"/>
     </row>
-    <row r="100" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>156</v>
       </c>
@@ -10251,7 +10253,7 @@
       <c r="BO100" s="11"/>
       <c r="BP100" s="2"/>
     </row>
-    <row r="101" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>156</v>
       </c>
@@ -10341,7 +10343,7 @@
       <c r="BO101" s="11"/>
       <c r="BP101" s="2"/>
     </row>
-    <row r="102" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>156</v>
       </c>
@@ -10431,7 +10433,7 @@
       <c r="BO102" s="11"/>
       <c r="BP102" s="2"/>
     </row>
-    <row r="103" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>156</v>
       </c>
@@ -10521,7 +10523,7 @@
       <c r="BO103" s="11"/>
       <c r="BP103" s="2"/>
     </row>
-    <row r="104" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>156</v>
       </c>
@@ -10611,7 +10613,7 @@
       <c r="BO104" s="11"/>
       <c r="BP104" s="2"/>
     </row>
-    <row r="105" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>156</v>
       </c>
@@ -10701,12 +10703,12 @@
       <c r="BO105" s="11"/>
       <c r="BP105" s="2"/>
     </row>
-    <row r="106" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="15"/>
@@ -10777,7 +10779,7 @@
       <c r="BO106" s="29"/>
       <c r="BP106" s="2"/>
     </row>
-    <row r="107" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B107" s="2" t="s">
         <v>17</v>
       </c>
@@ -10867,7 +10869,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="108" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B108" s="2" t="s">
         <v>18</v>
       </c>
@@ -10941,78 +10943,77 @@
       <c r="BO108" s="11"/>
       <c r="BP108" s="2"/>
     </row>
-    <row r="109" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="10"/>
-      <c r="G109" s="10"/>
-      <c r="H109" s="10"/>
-      <c r="I109" s="10"/>
-      <c r="J109" s="10"/>
-      <c r="K109" s="10"/>
-      <c r="L109" s="10"/>
-      <c r="M109" s="10"/>
-      <c r="N109" s="10"/>
-      <c r="O109" s="10"/>
-      <c r="P109" s="10"/>
-      <c r="Q109" s="10"/>
-      <c r="R109" s="10"/>
-      <c r="S109" s="10"/>
-      <c r="T109" s="10"/>
-      <c r="U109" s="10"/>
-      <c r="V109" s="10"/>
-      <c r="W109" s="10"/>
-      <c r="X109" s="10"/>
-      <c r="Y109" s="10"/>
-      <c r="Z109" s="10"/>
-      <c r="AA109" s="10"/>
-      <c r="AB109" s="10"/>
-      <c r="AC109" s="10"/>
-      <c r="AD109" s="10"/>
-      <c r="AE109" s="10"/>
-      <c r="AF109" s="10"/>
-      <c r="AG109" s="10"/>
-      <c r="AH109" s="10"/>
-      <c r="AI109" s="10"/>
-      <c r="AJ109" s="10"/>
-      <c r="AK109" s="10"/>
-      <c r="AL109" s="10"/>
-      <c r="AM109" s="10"/>
-      <c r="AN109" s="10"/>
-      <c r="AO109" s="10"/>
-      <c r="AP109" s="10"/>
-      <c r="AQ109" s="10"/>
-      <c r="AR109" s="10"/>
-      <c r="AS109" s="10"/>
-      <c r="AT109" s="10"/>
-      <c r="AU109" s="10"/>
-      <c r="AV109" s="10"/>
-      <c r="AW109" s="10"/>
-      <c r="AX109" s="10"/>
-      <c r="AY109" s="10"/>
-      <c r="AZ109" s="10"/>
-      <c r="BA109" s="10"/>
-      <c r="BB109" s="10"/>
-      <c r="BC109" s="10"/>
-      <c r="BD109" s="18"/>
-      <c r="BE109" s="18"/>
-      <c r="BF109" s="18"/>
-      <c r="BG109" s="18"/>
-      <c r="BH109" s="18"/>
-      <c r="BI109" s="18"/>
-      <c r="BJ109" s="18"/>
-      <c r="BK109" s="18"/>
-      <c r="BL109" s="18"/>
-      <c r="BM109" s="18"/>
-      <c r="BN109" s="18"/>
-      <c r="BO109" s="18"/>
-      <c r="BP109" s="10"/>
-      <c r="BQ109" s="9"/>
-    </row>
-    <row r="110" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:68" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="31"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="31"/>
+      <c r="E109" s="31"/>
+      <c r="F109" s="31"/>
+      <c r="G109" s="31"/>
+      <c r="H109" s="31"/>
+      <c r="I109" s="31"/>
+      <c r="J109" s="31"/>
+      <c r="K109" s="31"/>
+      <c r="L109" s="31"/>
+      <c r="M109" s="31"/>
+      <c r="N109" s="31"/>
+      <c r="O109" s="31"/>
+      <c r="P109" s="31"/>
+      <c r="Q109" s="31"/>
+      <c r="R109" s="31"/>
+      <c r="S109" s="31"/>
+      <c r="T109" s="31"/>
+      <c r="U109" s="31"/>
+      <c r="V109" s="31"/>
+      <c r="W109" s="31"/>
+      <c r="X109" s="31"/>
+      <c r="Y109" s="31"/>
+      <c r="Z109" s="31"/>
+      <c r="AA109" s="31"/>
+      <c r="AB109" s="31"/>
+      <c r="AC109" s="31"/>
+      <c r="AD109" s="31"/>
+      <c r="AE109" s="31"/>
+      <c r="AF109" s="31"/>
+      <c r="AG109" s="31"/>
+      <c r="AH109" s="31"/>
+      <c r="AI109" s="31"/>
+      <c r="AJ109" s="31"/>
+      <c r="AK109" s="31"/>
+      <c r="AL109" s="31"/>
+      <c r="AM109" s="31"/>
+      <c r="AN109" s="31"/>
+      <c r="AO109" s="31"/>
+      <c r="AP109" s="31"/>
+      <c r="AQ109" s="31"/>
+      <c r="AR109" s="31"/>
+      <c r="AS109" s="31"/>
+      <c r="AT109" s="31"/>
+      <c r="AU109" s="31"/>
+      <c r="AV109" s="31"/>
+      <c r="AW109" s="31"/>
+      <c r="AX109" s="31"/>
+      <c r="AY109" s="31"/>
+      <c r="AZ109" s="31"/>
+      <c r="BA109" s="31"/>
+      <c r="BB109" s="31"/>
+      <c r="BC109" s="31"/>
+      <c r="BD109" s="36"/>
+      <c r="BE109" s="36"/>
+      <c r="BF109" s="36"/>
+      <c r="BG109" s="36"/>
+      <c r="BH109" s="36"/>
+      <c r="BI109" s="36"/>
+      <c r="BJ109" s="36"/>
+      <c r="BK109" s="36"/>
+      <c r="BL109" s="36"/>
+      <c r="BM109" s="36"/>
+      <c r="BN109" s="36"/>
+      <c r="BO109" s="36"/>
+      <c r="BP109" s="31"/>
+    </row>
+    <row r="110" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>158</v>
       </c>
@@ -11110,7 +11111,7 @@
       <c r="BO110" s="11"/>
       <c r="BP110" s="2"/>
     </row>
-    <row r="111" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>158</v>
       </c>
@@ -11200,7 +11201,7 @@
       <c r="BO111" s="11"/>
       <c r="BP111" s="2"/>
     </row>
-    <row r="112" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>158</v>
       </c>
@@ -11565,7 +11566,7 @@
         <v>158</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
@@ -12438,7 +12439,7 @@
         <v>160</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -13215,7 +13216,7 @@
         <v>162</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
@@ -13988,7 +13989,7 @@
         <v>163</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
@@ -14948,7 +14949,7 @@
         <v>165</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
@@ -15455,7 +15456,7 @@
       <c r="BO160" s="11"/>
       <c r="BP160" s="2"/>
     </row>
-    <row r="161" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>167</v>
       </c>
@@ -15545,7 +15546,7 @@
       <c r="BO161" s="11"/>
       <c r="BP161" s="2"/>
     </row>
-    <row r="162" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>167</v>
       </c>
@@ -15635,7 +15636,7 @@
       <c r="BO162" s="11"/>
       <c r="BP162" s="2"/>
     </row>
-    <row r="163" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>167</v>
       </c>
@@ -15725,7 +15726,7 @@
       <c r="BO163" s="11"/>
       <c r="BP163" s="2"/>
     </row>
-    <row r="164" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>167</v>
       </c>
@@ -15815,7 +15816,7 @@
       <c r="BO164" s="11"/>
       <c r="BP164" s="2"/>
     </row>
-    <row r="165" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>167</v>
       </c>
@@ -15905,7 +15906,7 @@
       <c r="BO165" s="11"/>
       <c r="BP165" s="2"/>
     </row>
-    <row r="166" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
         <v>167</v>
       </c>
@@ -15995,7 +15996,7 @@
       <c r="BO166" s="11"/>
       <c r="BP166" s="2"/>
     </row>
-    <row r="167" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>167</v>
       </c>
@@ -16085,7 +16086,7 @@
       <c r="BO167" s="11"/>
       <c r="BP167" s="2"/>
     </row>
-    <row r="168" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
@@ -16175,7 +16176,7 @@
       <c r="BO168" s="11"/>
       <c r="BP168" s="2"/>
     </row>
-    <row r="169" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>167</v>
       </c>
@@ -16265,12 +16266,12 @@
       <c r="BO169" s="11"/>
       <c r="BP169" s="2"/>
     </row>
-    <row r="170" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
@@ -16341,7 +16342,7 @@
       <c r="BO170" s="29"/>
       <c r="BP170" s="2"/>
     </row>
-    <row r="171" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B171" s="2" t="s">
         <v>17</v>
       </c>
@@ -16440,7 +16441,7 @@
         <v>3193</v>
       </c>
     </row>
-    <row r="172" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B172" s="2" t="s">
         <v>18</v>
       </c>
@@ -16514,78 +16515,77 @@
       <c r="BO172" s="11"/>
       <c r="BP172" s="2"/>
     </row>
-    <row r="173" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A173" s="10"/>
-      <c r="B173" s="10"/>
-      <c r="C173" s="10"/>
-      <c r="D173" s="10"/>
-      <c r="E173" s="10"/>
-      <c r="F173" s="10"/>
-      <c r="G173" s="10"/>
-      <c r="H173" s="10"/>
-      <c r="I173" s="10"/>
-      <c r="J173" s="10"/>
-      <c r="K173" s="10"/>
-      <c r="L173" s="10"/>
-      <c r="M173" s="10"/>
-      <c r="N173" s="10"/>
-      <c r="O173" s="10"/>
-      <c r="P173" s="10"/>
-      <c r="Q173" s="10"/>
-      <c r="R173" s="10"/>
-      <c r="S173" s="10"/>
-      <c r="T173" s="10"/>
-      <c r="U173" s="10"/>
-      <c r="V173" s="10"/>
-      <c r="W173" s="10"/>
-      <c r="X173" s="10"/>
-      <c r="Y173" s="10"/>
-      <c r="Z173" s="10"/>
-      <c r="AA173" s="10"/>
-      <c r="AB173" s="10"/>
-      <c r="AC173" s="10"/>
-      <c r="AD173" s="10"/>
-      <c r="AE173" s="10"/>
-      <c r="AF173" s="10"/>
-      <c r="AG173" s="10"/>
-      <c r="AH173" s="10"/>
-      <c r="AI173" s="10"/>
-      <c r="AJ173" s="10"/>
-      <c r="AK173" s="10"/>
-      <c r="AL173" s="10"/>
-      <c r="AM173" s="10"/>
-      <c r="AN173" s="10"/>
-      <c r="AO173" s="10"/>
-      <c r="AP173" s="10"/>
-      <c r="AQ173" s="10"/>
-      <c r="AR173" s="10"/>
-      <c r="AS173" s="10"/>
-      <c r="AT173" s="10"/>
-      <c r="AU173" s="10"/>
-      <c r="AV173" s="10"/>
-      <c r="AW173" s="10"/>
-      <c r="AX173" s="10"/>
-      <c r="AY173" s="10"/>
-      <c r="AZ173" s="10"/>
-      <c r="BA173" s="10"/>
-      <c r="BB173" s="10"/>
-      <c r="BC173" s="10"/>
-      <c r="BD173" s="18"/>
-      <c r="BE173" s="18"/>
-      <c r="BF173" s="18"/>
-      <c r="BG173" s="18"/>
-      <c r="BH173" s="18"/>
-      <c r="BI173" s="18"/>
-      <c r="BJ173" s="18"/>
-      <c r="BK173" s="18"/>
-      <c r="BL173" s="18"/>
-      <c r="BM173" s="18"/>
-      <c r="BN173" s="18"/>
-      <c r="BO173" s="18"/>
-      <c r="BP173" s="10"/>
-      <c r="BQ173" s="9"/>
-    </row>
-    <row r="174" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:68" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="31"/>
+      <c r="B173" s="31"/>
+      <c r="C173" s="31"/>
+      <c r="D173" s="31"/>
+      <c r="E173" s="31"/>
+      <c r="F173" s="31"/>
+      <c r="G173" s="31"/>
+      <c r="H173" s="31"/>
+      <c r="I173" s="31"/>
+      <c r="J173" s="31"/>
+      <c r="K173" s="31"/>
+      <c r="L173" s="31"/>
+      <c r="M173" s="31"/>
+      <c r="N173" s="31"/>
+      <c r="O173" s="31"/>
+      <c r="P173" s="31"/>
+      <c r="Q173" s="31"/>
+      <c r="R173" s="31"/>
+      <c r="S173" s="31"/>
+      <c r="T173" s="31"/>
+      <c r="U173" s="31"/>
+      <c r="V173" s="31"/>
+      <c r="W173" s="31"/>
+      <c r="X173" s="31"/>
+      <c r="Y173" s="31"/>
+      <c r="Z173" s="31"/>
+      <c r="AA173" s="31"/>
+      <c r="AB173" s="31"/>
+      <c r="AC173" s="31"/>
+      <c r="AD173" s="31"/>
+      <c r="AE173" s="31"/>
+      <c r="AF173" s="31"/>
+      <c r="AG173" s="31"/>
+      <c r="AH173" s="31"/>
+      <c r="AI173" s="31"/>
+      <c r="AJ173" s="31"/>
+      <c r="AK173" s="31"/>
+      <c r="AL173" s="31"/>
+      <c r="AM173" s="31"/>
+      <c r="AN173" s="31"/>
+      <c r="AO173" s="31"/>
+      <c r="AP173" s="31"/>
+      <c r="AQ173" s="31"/>
+      <c r="AR173" s="31"/>
+      <c r="AS173" s="31"/>
+      <c r="AT173" s="31"/>
+      <c r="AU173" s="31"/>
+      <c r="AV173" s="31"/>
+      <c r="AW173" s="31"/>
+      <c r="AX173" s="31"/>
+      <c r="AY173" s="31"/>
+      <c r="AZ173" s="31"/>
+      <c r="BA173" s="31"/>
+      <c r="BB173" s="31"/>
+      <c r="BC173" s="31"/>
+      <c r="BD173" s="36"/>
+      <c r="BE173" s="36"/>
+      <c r="BF173" s="36"/>
+      <c r="BG173" s="36"/>
+      <c r="BH173" s="36"/>
+      <c r="BI173" s="36"/>
+      <c r="BJ173" s="36"/>
+      <c r="BK173" s="36"/>
+      <c r="BL173" s="36"/>
+      <c r="BM173" s="36"/>
+      <c r="BN173" s="36"/>
+      <c r="BO173" s="36"/>
+      <c r="BP173" s="31"/>
+    </row>
+    <row r="174" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
         <v>169</v>
       </c>
@@ -16685,7 +16685,7 @@
       <c r="BO174" s="11"/>
       <c r="BP174" s="2"/>
     </row>
-    <row r="175" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>169</v>
       </c>
@@ -16783,7 +16783,7 @@
       <c r="BO175" s="11"/>
       <c r="BP175" s="2"/>
     </row>
-    <row r="176" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
         <v>169</v>
       </c>
@@ -17328,7 +17328,7 @@
         <v>169</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
@@ -18200,7 +18200,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="8"/>
@@ -19259,7 +19259,7 @@
         <v>171</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="8"/>
@@ -20122,7 +20122,7 @@
         <v>175</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="8"/>
@@ -20891,7 +20891,7 @@
         <v>180</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C223" s="8"/>
       <c r="D223" s="8"/>
@@ -21569,7 +21569,7 @@
         <v>181</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C231" s="8"/>
       <c r="D231" s="8"/>
@@ -21809,76 +21809,75 @@
       <c r="BO233" s="11"/>
       <c r="BP233" s="2"/>
     </row>
-    <row r="234" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A234" s="10"/>
-      <c r="B234" s="10"/>
-      <c r="C234" s="10"/>
-      <c r="D234" s="10"/>
-      <c r="E234" s="10"/>
-      <c r="F234" s="10"/>
-      <c r="G234" s="10"/>
-      <c r="H234" s="10"/>
-      <c r="I234" s="10"/>
-      <c r="J234" s="10"/>
-      <c r="K234" s="10"/>
-      <c r="L234" s="10"/>
-      <c r="M234" s="10"/>
-      <c r="N234" s="10"/>
-      <c r="O234" s="10"/>
-      <c r="P234" s="10"/>
-      <c r="Q234" s="10"/>
-      <c r="R234" s="10"/>
-      <c r="S234" s="10"/>
-      <c r="T234" s="10"/>
-      <c r="U234" s="10"/>
-      <c r="V234" s="10"/>
-      <c r="W234" s="10"/>
-      <c r="X234" s="10"/>
-      <c r="Y234" s="10"/>
-      <c r="Z234" s="10"/>
-      <c r="AA234" s="10"/>
-      <c r="AB234" s="10"/>
-      <c r="AC234" s="10"/>
-      <c r="AD234" s="10"/>
-      <c r="AE234" s="10"/>
-      <c r="AF234" s="10"/>
-      <c r="AG234" s="10"/>
-      <c r="AH234" s="10"/>
-      <c r="AI234" s="10"/>
-      <c r="AJ234" s="10"/>
-      <c r="AK234" s="10"/>
-      <c r="AL234" s="10"/>
-      <c r="AM234" s="10"/>
-      <c r="AN234" s="10"/>
-      <c r="AO234" s="10"/>
-      <c r="AP234" s="10"/>
-      <c r="AQ234" s="10"/>
-      <c r="AR234" s="10"/>
-      <c r="AS234" s="10"/>
-      <c r="AT234" s="10"/>
-      <c r="AU234" s="10"/>
-      <c r="AV234" s="10"/>
-      <c r="AW234" s="10"/>
-      <c r="AX234" s="10"/>
-      <c r="AY234" s="10"/>
-      <c r="AZ234" s="10"/>
-      <c r="BA234" s="10"/>
-      <c r="BB234" s="10"/>
-      <c r="BC234" s="10"/>
-      <c r="BD234" s="18"/>
-      <c r="BE234" s="18"/>
-      <c r="BF234" s="18"/>
-      <c r="BG234" s="18"/>
-      <c r="BH234" s="18"/>
-      <c r="BI234" s="18"/>
-      <c r="BJ234" s="18"/>
-      <c r="BK234" s="18"/>
-      <c r="BL234" s="18"/>
-      <c r="BM234" s="18"/>
-      <c r="BN234" s="18"/>
-      <c r="BO234" s="18"/>
-      <c r="BP234" s="10"/>
-      <c r="BQ234" s="9"/>
+    <row r="234" spans="1:69" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A234" s="31"/>
+      <c r="B234" s="31"/>
+      <c r="C234" s="31"/>
+      <c r="D234" s="31"/>
+      <c r="E234" s="31"/>
+      <c r="F234" s="31"/>
+      <c r="G234" s="31"/>
+      <c r="H234" s="31"/>
+      <c r="I234" s="31"/>
+      <c r="J234" s="31"/>
+      <c r="K234" s="31"/>
+      <c r="L234" s="31"/>
+      <c r="M234" s="31"/>
+      <c r="N234" s="31"/>
+      <c r="O234" s="31"/>
+      <c r="P234" s="31"/>
+      <c r="Q234" s="31"/>
+      <c r="R234" s="31"/>
+      <c r="S234" s="31"/>
+      <c r="T234" s="31"/>
+      <c r="U234" s="31"/>
+      <c r="V234" s="31"/>
+      <c r="W234" s="31"/>
+      <c r="X234" s="31"/>
+      <c r="Y234" s="31"/>
+      <c r="Z234" s="31"/>
+      <c r="AA234" s="31"/>
+      <c r="AB234" s="31"/>
+      <c r="AC234" s="31"/>
+      <c r="AD234" s="31"/>
+      <c r="AE234" s="31"/>
+      <c r="AF234" s="31"/>
+      <c r="AG234" s="31"/>
+      <c r="AH234" s="31"/>
+      <c r="AI234" s="31"/>
+      <c r="AJ234" s="31"/>
+      <c r="AK234" s="31"/>
+      <c r="AL234" s="31"/>
+      <c r="AM234" s="31"/>
+      <c r="AN234" s="31"/>
+      <c r="AO234" s="31"/>
+      <c r="AP234" s="31"/>
+      <c r="AQ234" s="31"/>
+      <c r="AR234" s="31"/>
+      <c r="AS234" s="31"/>
+      <c r="AT234" s="31"/>
+      <c r="AU234" s="31"/>
+      <c r="AV234" s="31"/>
+      <c r="AW234" s="31"/>
+      <c r="AX234" s="31"/>
+      <c r="AY234" s="31"/>
+      <c r="AZ234" s="31"/>
+      <c r="BA234" s="31"/>
+      <c r="BB234" s="31"/>
+      <c r="BC234" s="31"/>
+      <c r="BD234" s="36"/>
+      <c r="BE234" s="36"/>
+      <c r="BF234" s="36"/>
+      <c r="BG234" s="36"/>
+      <c r="BH234" s="36"/>
+      <c r="BI234" s="36"/>
+      <c r="BJ234" s="36"/>
+      <c r="BK234" s="36"/>
+      <c r="BL234" s="36"/>
+      <c r="BM234" s="36"/>
+      <c r="BN234" s="36"/>
+      <c r="BO234" s="36"/>
+      <c r="BP234" s="31"/>
     </row>
     <row r="235" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
@@ -22429,7 +22428,7 @@
         <v>183</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C241" s="8"/>
       <c r="D241" s="8"/>
@@ -23199,7 +23198,7 @@
         <v>185</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C250" s="8"/>
       <c r="D250" s="8"/>
@@ -24239,7 +24238,7 @@
         <v>186</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C262" s="8"/>
       <c r="D262" s="8"/>
@@ -24919,7 +24918,7 @@
         <v>187</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C270" s="8"/>
       <c r="D270" s="8"/>
@@ -25157,7 +25156,7 @@
       <c r="BO272" s="11"/>
       <c r="BP272" s="2"/>
     </row>
-    <row r="273" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -25226,7 +25225,7 @@
       <c r="BO273" s="11"/>
       <c r="BP273" s="2"/>
     </row>
-    <row r="274" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
         <v>188</v>
       </c>
@@ -25324,7 +25323,7 @@
       <c r="BO274" s="11"/>
       <c r="BP274" s="2"/>
     </row>
-    <row r="275" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
         <v>188</v>
       </c>
@@ -25414,7 +25413,7 @@
       <c r="BO275" s="11"/>
       <c r="BP275" s="2"/>
     </row>
-    <row r="276" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
         <v>188</v>
       </c>
@@ -25504,7 +25503,7 @@
       <c r="BO276" s="11"/>
       <c r="BP276" s="2"/>
     </row>
-    <row r="277" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
         <v>188</v>
       </c>
@@ -25594,12 +25593,12 @@
       <c r="BO277" s="11"/>
       <c r="BP277" s="2"/>
     </row>
-    <row r="278" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C278" s="8"/>
       <c r="D278" s="8"/>
@@ -25670,7 +25669,7 @@
       <c r="BO278" s="29"/>
       <c r="BP278" s="2"/>
     </row>
-    <row r="279" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B279" s="2" t="s">
         <v>17</v>
       </c>
@@ -25763,7 +25762,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="280" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B280" s="2" t="s">
         <v>18</v>
       </c>
@@ -25837,7 +25836,7 @@
       <c r="BO280" s="11"/>
       <c r="BP280" s="2"/>
     </row>
-    <row r="281" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -25906,7 +25905,7 @@
       <c r="BO281" s="11"/>
       <c r="BP281" s="2"/>
     </row>
-    <row r="282" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
         <v>190</v>
       </c>
@@ -26004,7 +26003,7 @@
       <c r="BO282" s="11"/>
       <c r="BP282" s="2"/>
     </row>
-    <row r="283" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A283" s="2" t="s">
         <v>190</v>
       </c>
@@ -26094,7 +26093,7 @@
       <c r="BO283" s="11"/>
       <c r="BP283" s="2"/>
     </row>
-    <row r="284" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
         <v>190</v>
       </c>
@@ -26184,12 +26183,12 @@
       <c r="BO284" s="11"/>
       <c r="BP284" s="2"/>
     </row>
-    <row r="285" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A285" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C285" s="8"/>
       <c r="D285" s="8"/>
@@ -26260,7 +26259,7 @@
       <c r="BO285" s="29"/>
       <c r="BP285" s="2"/>
     </row>
-    <row r="286" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2">
@@ -26351,7 +26350,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="287" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -26423,76 +26422,75 @@
       <c r="BO287" s="11"/>
       <c r="BP287" s="2"/>
     </row>
-    <row r="288" spans="1:69" x14ac:dyDescent="0.35">
-      <c r="A288" s="10"/>
-      <c r="B288" s="10"/>
-      <c r="C288" s="10"/>
-      <c r="D288" s="10"/>
-      <c r="E288" s="10"/>
-      <c r="F288" s="10"/>
-      <c r="G288" s="10"/>
-      <c r="H288" s="10"/>
-      <c r="I288" s="10"/>
-      <c r="J288" s="10"/>
-      <c r="K288" s="10"/>
-      <c r="L288" s="10"/>
-      <c r="M288" s="10"/>
-      <c r="N288" s="10"/>
-      <c r="O288" s="10"/>
-      <c r="P288" s="10"/>
-      <c r="Q288" s="10"/>
-      <c r="R288" s="10"/>
-      <c r="S288" s="10"/>
-      <c r="T288" s="10"/>
-      <c r="U288" s="10"/>
-      <c r="V288" s="10"/>
-      <c r="W288" s="10"/>
-      <c r="X288" s="10"/>
-      <c r="Y288" s="10"/>
-      <c r="Z288" s="10"/>
-      <c r="AA288" s="10"/>
-      <c r="AB288" s="10"/>
-      <c r="AC288" s="10"/>
-      <c r="AD288" s="10"/>
-      <c r="AE288" s="10"/>
-      <c r="AF288" s="10"/>
-      <c r="AG288" s="10"/>
-      <c r="AH288" s="10"/>
-      <c r="AI288" s="10"/>
-      <c r="AJ288" s="10"/>
-      <c r="AK288" s="10"/>
-      <c r="AL288" s="10"/>
-      <c r="AM288" s="10"/>
-      <c r="AN288" s="10"/>
-      <c r="AO288" s="10"/>
-      <c r="AP288" s="10"/>
-      <c r="AQ288" s="10"/>
-      <c r="AR288" s="10"/>
-      <c r="AS288" s="10"/>
-      <c r="AT288" s="10"/>
-      <c r="AU288" s="10"/>
-      <c r="AV288" s="10"/>
-      <c r="AW288" s="10"/>
-      <c r="AX288" s="10"/>
-      <c r="AY288" s="10"/>
-      <c r="AZ288" s="10"/>
-      <c r="BA288" s="10"/>
-      <c r="BB288" s="10"/>
-      <c r="BC288" s="10"/>
-      <c r="BD288" s="18"/>
-      <c r="BE288" s="18"/>
-      <c r="BF288" s="18"/>
-      <c r="BG288" s="18"/>
-      <c r="BH288" s="18"/>
-      <c r="BI288" s="18"/>
-      <c r="BJ288" s="18"/>
-      <c r="BK288" s="18"/>
-      <c r="BL288" s="18"/>
-      <c r="BM288" s="18"/>
-      <c r="BN288" s="18"/>
-      <c r="BO288" s="18"/>
-      <c r="BP288" s="10"/>
-      <c r="BQ288" s="9"/>
+    <row r="288" spans="1:68" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A288" s="31"/>
+      <c r="B288" s="31"/>
+      <c r="C288" s="31"/>
+      <c r="D288" s="31"/>
+      <c r="E288" s="31"/>
+      <c r="F288" s="31"/>
+      <c r="G288" s="31"/>
+      <c r="H288" s="31"/>
+      <c r="I288" s="31"/>
+      <c r="J288" s="31"/>
+      <c r="K288" s="31"/>
+      <c r="L288" s="31"/>
+      <c r="M288" s="31"/>
+      <c r="N288" s="31"/>
+      <c r="O288" s="31"/>
+      <c r="P288" s="31"/>
+      <c r="Q288" s="31"/>
+      <c r="R288" s="31"/>
+      <c r="S288" s="31"/>
+      <c r="T288" s="31"/>
+      <c r="U288" s="31"/>
+      <c r="V288" s="31"/>
+      <c r="W288" s="31"/>
+      <c r="X288" s="31"/>
+      <c r="Y288" s="31"/>
+      <c r="Z288" s="31"/>
+      <c r="AA288" s="31"/>
+      <c r="AB288" s="31"/>
+      <c r="AC288" s="31"/>
+      <c r="AD288" s="31"/>
+      <c r="AE288" s="31"/>
+      <c r="AF288" s="31"/>
+      <c r="AG288" s="31"/>
+      <c r="AH288" s="31"/>
+      <c r="AI288" s="31"/>
+      <c r="AJ288" s="31"/>
+      <c r="AK288" s="31"/>
+      <c r="AL288" s="31"/>
+      <c r="AM288" s="31"/>
+      <c r="AN288" s="31"/>
+      <c r="AO288" s="31"/>
+      <c r="AP288" s="31"/>
+      <c r="AQ288" s="31"/>
+      <c r="AR288" s="31"/>
+      <c r="AS288" s="31"/>
+      <c r="AT288" s="31"/>
+      <c r="AU288" s="31"/>
+      <c r="AV288" s="31"/>
+      <c r="AW288" s="31"/>
+      <c r="AX288" s="31"/>
+      <c r="AY288" s="31"/>
+      <c r="AZ288" s="31"/>
+      <c r="BA288" s="31"/>
+      <c r="BB288" s="31"/>
+      <c r="BC288" s="31"/>
+      <c r="BD288" s="36"/>
+      <c r="BE288" s="36"/>
+      <c r="BF288" s="36"/>
+      <c r="BG288" s="36"/>
+      <c r="BH288" s="36"/>
+      <c r="BI288" s="36"/>
+      <c r="BJ288" s="36"/>
+      <c r="BK288" s="36"/>
+      <c r="BL288" s="36"/>
+      <c r="BM288" s="36"/>
+      <c r="BN288" s="36"/>
+      <c r="BO288" s="36"/>
+      <c r="BP288" s="31"/>
     </row>
     <row r="289" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A289" s="2" t="s">
@@ -27229,7 +27227,7 @@
         <v>191</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C297" s="8"/>
       <c r="D297" s="8"/>
@@ -27911,7 +27909,7 @@
         <v>192</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C305" s="8"/>
       <c r="D305" s="8"/>
@@ -28777,7 +28775,7 @@
         <v>193</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C315" s="8"/>
       <c r="D315" s="8"/>
@@ -29554,7 +29552,7 @@
         <v>194</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C324" s="8"/>
       <c r="D324" s="8"/>
@@ -30706,7 +30704,7 @@
         <v>195</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C337" s="8"/>
       <c r="D337" s="8"/>
@@ -31576,7 +31574,7 @@
         <v>199</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C347" s="8"/>
       <c r="D347" s="8"/>
@@ -32269,7 +32267,7 @@
         <v>19</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I360">
         <v>8774.25</v>
@@ -32662,7 +32660,7 @@
         <v>20</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I368">
         <v>7451.2</v>
@@ -33103,7 +33101,7 @@
         <v>24</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I378">
         <v>10113.75</v>
@@ -33468,7 +33466,7 @@
         <v>27</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I386">
         <v>5961.3</v>
@@ -33809,7 +33807,7 @@
         <v>29</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I396">
         <v>9131.4500000000007</v>
@@ -34190,7 +34188,7 @@
         <v>38</v>
       </c>
       <c r="B408" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I408" s="7">
         <v>8358.2999999999993</v>
@@ -34272,75 +34270,9 @@
       <c r="BN410" s="2"/>
       <c r="BP410" s="2"/>
     </row>
-    <row r="411" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A411" s="10"/>
-      <c r="B411" s="9"/>
-      <c r="C411" s="9"/>
-      <c r="D411" s="9"/>
-      <c r="E411" s="9"/>
-      <c r="F411" s="9"/>
-      <c r="G411" s="9"/>
-      <c r="H411" s="9"/>
-      <c r="I411" s="9"/>
-      <c r="J411" s="9"/>
-      <c r="K411" s="9"/>
-      <c r="L411" s="9"/>
-      <c r="M411" s="9"/>
-      <c r="N411" s="9"/>
-      <c r="O411" s="9"/>
-      <c r="P411" s="9"/>
-      <c r="Q411" s="9"/>
-      <c r="R411" s="9"/>
-      <c r="S411" s="9"/>
-      <c r="T411" s="9"/>
-      <c r="U411" s="9"/>
-      <c r="V411" s="9"/>
-      <c r="W411" s="9"/>
-      <c r="X411" s="9"/>
-      <c r="Y411" s="9"/>
-      <c r="Z411" s="9"/>
-      <c r="AA411" s="9"/>
-      <c r="AB411" s="9"/>
-      <c r="AC411" s="9"/>
-      <c r="AD411" s="9"/>
-      <c r="AE411" s="9"/>
-      <c r="AF411" s="9"/>
-      <c r="AG411" s="9"/>
-      <c r="AH411" s="9"/>
-      <c r="AI411" s="9"/>
-      <c r="AJ411" s="9"/>
-      <c r="AK411" s="9"/>
-      <c r="AL411" s="9"/>
-      <c r="AM411" s="9"/>
-      <c r="AN411" s="9"/>
-      <c r="AO411" s="9"/>
-      <c r="AP411" s="9"/>
-      <c r="AQ411" s="9"/>
-      <c r="AR411" s="9"/>
-      <c r="AS411" s="9"/>
-      <c r="AT411" s="9"/>
-      <c r="AU411" s="9"/>
-      <c r="AV411" s="9"/>
-      <c r="AW411" s="9"/>
-      <c r="AX411" s="9"/>
-      <c r="AY411" s="9"/>
-      <c r="AZ411" s="9"/>
-      <c r="BA411" s="9"/>
-      <c r="BB411" s="9"/>
-      <c r="BC411" s="9"/>
-      <c r="BD411" s="9"/>
-      <c r="BE411" s="9"/>
-      <c r="BF411" s="9"/>
-      <c r="BG411" s="9"/>
-      <c r="BH411" s="9"/>
-      <c r="BI411" s="9"/>
-      <c r="BJ411" s="9"/>
-      <c r="BK411" s="9"/>
-      <c r="BL411" s="9"/>
-      <c r="BM411" s="9"/>
-      <c r="BN411" s="9"/>
-      <c r="BO411" s="9"/>
-      <c r="BP411" s="13"/>
+    <row r="411" spans="1:68" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A411" s="31"/>
+      <c r="BP411" s="31"/>
     </row>
     <row r="412" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A412" s="2" t="s">
@@ -34669,7 +34601,7 @@
         <v>90</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I422">
         <v>19524.7</v>
@@ -35166,7 +35098,7 @@
         <v>177</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I439">
         <v>19217.349999999999</v>
@@ -35411,7 +35343,7 @@
         <v>220</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I450">
         <v>11786.95</v>
@@ -35662,7 +35594,7 @@
         <v>246</v>
       </c>
       <c r="B462" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H462" s="6"/>
       <c r="I462">
@@ -36119,7 +36051,7 @@
         <v>250</v>
       </c>
       <c r="B478" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I478">
         <v>13790.3</v>
@@ -36425,7 +36357,7 @@
         <v>254</v>
       </c>
       <c r="B490" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I490">
         <v>17450</v>
@@ -36468,7 +36400,7 @@
     <row r="493" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="494" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A494" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B494" t="s">
         <v>8</v>
@@ -36502,7 +36434,7 @@
     </row>
     <row r="495" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A495" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B495" s="8" t="s">
         <v>14</v>
@@ -36533,7 +36465,7 @@
     </row>
     <row r="496" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A496" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B496" s="8" t="s">
         <v>15</v>
@@ -36564,7 +36496,7 @@
     </row>
     <row r="497" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A497" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B497" s="8" t="s">
         <v>26</v>
@@ -36595,10 +36527,10 @@
     </row>
     <row r="498" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A498" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B498" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I498" s="14">
         <v>8253.15</v>
@@ -36641,7 +36573,7 @@
     </row>
     <row r="502" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A502" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B502" t="s">
         <v>14</v>
@@ -36670,13 +36602,16 @@
         <v>2560</v>
       </c>
     </row>
+    <row r="505" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A505" s="31"/>
+    </row>
+    <row r="506" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A506" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="BH1:BK1"/>
-    <mergeCell ref="BL1:BO1"/>
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="X1:AA1"/>
@@ -36686,6 +36621,11 @@
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="BH1:BK1"/>
+    <mergeCell ref="BL1:BO1"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AR1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -36694,11 +36634,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617BFE3A-5538-4FC4-A07C-C660CA12141D}">
-  <dimension ref="A1:M353"/>
+  <dimension ref="A1:M361"/>
   <sheetViews>
     <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L350" sqref="L350"/>
+      <pane ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E363" sqref="E363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36728,7 +36668,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
@@ -36738,7 +36678,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>129</v>
@@ -36747,7 +36687,7 @@
         <v>232</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -36755,7 +36695,7 @@
         <v>107</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" s="8">
         <v>200</v>
@@ -36843,7 +36783,7 @@
         <v>107</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C6" s="8">
         <f>(D6*E6)</f>
@@ -36865,7 +36805,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
@@ -36907,7 +36847,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C9" s="8">
         <v>200</v>
@@ -36995,7 +36935,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" s="8">
         <f>(D13*E13)</f>
@@ -37017,7 +36957,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
@@ -37059,7 +36999,7 @@
         <v>113</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C16" s="8">
         <v>200</v>
@@ -37147,7 +37087,7 @@
         <v>113</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C20" s="8">
         <f>(D20*E20)</f>
@@ -37169,7 +37109,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
@@ -37211,7 +37151,7 @@
         <v>131</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C23" s="8">
         <v>200</v>
@@ -37299,7 +37239,7 @@
         <v>131</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" s="8">
         <f>(D27*E27)</f>
@@ -37321,7 +37261,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
@@ -37363,7 +37303,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C30" s="8">
         <v>200</v>
@@ -37451,7 +37391,7 @@
         <v>134</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C34" s="8">
         <f>(D34*E34)</f>
@@ -37473,7 +37413,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2">
@@ -37529,7 +37469,7 @@
         <v>138</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C38" s="8">
         <v>200</v>
@@ -37617,7 +37557,7 @@
         <v>138</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C42" s="8">
         <f>(D42*E42)</f>
@@ -37639,7 +37579,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
@@ -37681,7 +37621,7 @@
         <v>142</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C45" s="8">
         <v>200</v>
@@ -37769,7 +37709,7 @@
         <v>142</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C49" s="8">
         <f>(D49*E49)</f>
@@ -37791,7 +37731,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2">
@@ -37833,7 +37773,7 @@
         <v>145</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C52" s="8">
         <v>200</v>
@@ -37921,7 +37861,7 @@
         <v>145</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C56" s="8">
         <f>(D56*E56)</f>
@@ -37943,7 +37883,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2">
@@ -37985,7 +37925,7 @@
         <v>149</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C59" s="8">
         <v>200</v>
@@ -38073,7 +38013,7 @@
         <v>149</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C63" s="8">
         <f>(D63*E63)</f>
@@ -38095,7 +38035,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2">
@@ -38137,7 +38077,7 @@
         <v>153</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C66" s="8">
         <v>200</v>
@@ -38225,7 +38165,7 @@
         <v>153</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C70" s="8">
         <f>(D70*E70)</f>
@@ -38247,7 +38187,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2">
@@ -38289,7 +38229,7 @@
         <v>156</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C73" s="8">
         <v>200</v>
@@ -38377,7 +38317,7 @@
         <v>156</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C77" s="8">
         <f>(D77*E77)</f>
@@ -38399,7 +38339,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2">
@@ -38455,7 +38395,7 @@
         <v>158</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C81" s="8">
         <v>200</v>
@@ -38543,7 +38483,7 @@
         <v>158</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C85" s="8">
         <f>(D85*E85)</f>
@@ -38565,7 +38505,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="2">
@@ -38607,7 +38547,7 @@
         <v>160</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C88" s="8">
         <v>200</v>
@@ -38695,7 +38635,7 @@
         <v>160</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C92" s="8">
         <f>(D92*E92)</f>
@@ -38717,7 +38657,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="2">
@@ -38759,7 +38699,7 @@
         <v>162</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C95" s="8">
         <v>200</v>
@@ -38847,7 +38787,7 @@
         <v>162</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C99" s="8">
         <f>(D99*E99)</f>
@@ -38869,7 +38809,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="2">
@@ -38911,7 +38851,7 @@
         <v>163</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C102" s="8">
         <v>200</v>
@@ -38999,7 +38939,7 @@
         <v>163</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C106" s="8">
         <f>(D106*E106)</f>
@@ -39021,7 +38961,7 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="2">
@@ -39063,7 +39003,7 @@
         <v>165</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C109" s="8">
         <v>200</v>
@@ -39151,7 +39091,7 @@
         <v>165</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C113" s="8">
         <f>(D113*E113)</f>
@@ -39173,7 +39113,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="2">
@@ -39215,7 +39155,7 @@
         <v>167</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C116" s="8">
         <v>200</v>
@@ -39303,7 +39243,7 @@
         <v>167</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C120" s="8">
         <f>(D120*E120)</f>
@@ -39325,7 +39265,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="2">
@@ -39381,7 +39321,7 @@
         <v>169</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C124" s="8">
         <v>200</v>
@@ -39469,7 +39409,7 @@
         <v>169</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C128" s="8">
         <f>(D128*E128)</f>
@@ -39491,7 +39431,7 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="2">
@@ -39533,7 +39473,7 @@
         <v>170</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C131" s="8">
         <v>200</v>
@@ -39621,7 +39561,7 @@
         <v>170</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C135" s="8">
         <f>(D135*E135)</f>
@@ -39643,7 +39583,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="2">
@@ -39685,7 +39625,7 @@
         <v>171</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C138" s="8">
         <v>200</v>
@@ -39773,7 +39713,7 @@
         <v>171</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C142" s="8">
         <f>(D142*E142)</f>
@@ -39795,7 +39735,7 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="2">
@@ -39837,7 +39777,7 @@
         <v>175</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C145" s="8">
         <v>200</v>
@@ -39925,7 +39865,7 @@
         <v>175</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C149" s="8">
         <f>(D149*E149)</f>
@@ -39947,7 +39887,7 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="2">
@@ -39989,7 +39929,7 @@
         <v>180</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C152" s="8">
         <v>200</v>
@@ -40077,7 +40017,7 @@
         <v>180</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C156" s="8">
         <f>(D156*E156)</f>
@@ -40099,7 +40039,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="2">
@@ -40141,7 +40081,7 @@
         <v>181</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C159" s="8">
         <v>200</v>
@@ -40229,7 +40169,7 @@
         <v>181</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C163" s="8">
         <f>(D163*E163)</f>
@@ -40251,7 +40191,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B164" s="8"/>
       <c r="C164" s="2">
@@ -40307,7 +40247,7 @@
         <v>183</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C167" s="8">
         <v>200</v>
@@ -40395,7 +40335,7 @@
         <v>183</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C171" s="8">
         <f>(D171*E171)</f>
@@ -40417,7 +40357,7 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B172" s="8"/>
       <c r="C172" s="2">
@@ -40459,7 +40399,7 @@
         <v>185</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C174" s="8">
         <v>200</v>
@@ -40547,7 +40487,7 @@
         <v>185</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C178" s="8">
         <f>(D178*E178)</f>
@@ -40569,7 +40509,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B179" s="8"/>
       <c r="C179" s="2">
@@ -40611,7 +40551,7 @@
         <v>186</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C181" s="8">
         <v>200</v>
@@ -40699,7 +40639,7 @@
         <v>186</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C185" s="8">
         <f>(D185*E185)</f>
@@ -40721,7 +40661,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="2">
@@ -40763,7 +40703,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C188" s="8">
         <v>200</v>
@@ -40851,7 +40791,7 @@
         <v>187</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C192" s="8">
         <f>(D192*E192)</f>
@@ -40873,7 +40813,7 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B193" s="8"/>
       <c r="C193" s="2">
@@ -40915,7 +40855,7 @@
         <v>188</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C195" s="8">
         <v>200</v>
@@ -41003,7 +40943,7 @@
         <v>188</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C199" s="8">
         <f>(D199*E199)</f>
@@ -41025,7 +40965,7 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B200" s="8"/>
       <c r="C200" s="2">
@@ -41067,7 +41007,7 @@
         <v>190</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C202" s="8">
         <v>200</v>
@@ -41155,7 +41095,7 @@
         <v>190</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C206" s="8">
         <f>(D206*E206)</f>
@@ -41177,7 +41117,7 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B207" s="8"/>
       <c r="C207" s="2">
@@ -41233,7 +41173,7 @@
         <v>191</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C210" s="8">
         <v>200</v>
@@ -41321,7 +41261,7 @@
         <v>191</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C214" s="8">
         <f>(D214*E214)</f>
@@ -41343,7 +41283,7 @@
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B215" s="8"/>
       <c r="C215" s="2">
@@ -41385,7 +41325,7 @@
         <v>192</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C217" s="8">
         <v>200</v>
@@ -41473,7 +41413,7 @@
         <v>192</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C221" s="8">
         <f>(D221*E221)</f>
@@ -41495,7 +41435,7 @@
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B222" s="8"/>
       <c r="C222" s="2">
@@ -41537,7 +41477,7 @@
         <v>193</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C224" s="8">
         <v>200</v>
@@ -41625,7 +41565,7 @@
         <v>193</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C228" s="8">
         <f>(D228*E228)</f>
@@ -41647,7 +41587,7 @@
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B229" s="8"/>
       <c r="C229" s="2">
@@ -41689,7 +41629,7 @@
         <v>194</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C231" s="8">
         <v>200</v>
@@ -41777,7 +41717,7 @@
         <v>194</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C235" s="8">
         <f>(D235*E235)</f>
@@ -41799,7 +41739,7 @@
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B236" s="8"/>
       <c r="C236" s="2">
@@ -41841,7 +41781,7 @@
         <v>195</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C238" s="8">
         <v>200</v>
@@ -41929,7 +41869,7 @@
         <v>195</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C242" s="8">
         <f>(D242*E242)</f>
@@ -41951,7 +41891,7 @@
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B243" s="8"/>
       <c r="C243" s="2">
@@ -41993,7 +41933,7 @@
         <v>199</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C245" s="8">
         <v>200</v>
@@ -42081,7 +42021,7 @@
         <v>199</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C249" s="8">
         <f>(D249*E249)</f>
@@ -42103,7 +42043,7 @@
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B250" s="8"/>
       <c r="C250" s="2">
@@ -42159,7 +42099,7 @@
         <v>19</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C253" s="8">
         <v>200</v>
@@ -42247,7 +42187,7 @@
         <v>19</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C257" s="8">
         <f>(D257*E257)</f>
@@ -42269,7 +42209,7 @@
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B258" s="8"/>
       <c r="C258" s="2">
@@ -42311,7 +42251,7 @@
         <v>20</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C260" s="8">
         <v>200</v>
@@ -42399,7 +42339,7 @@
         <v>20</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C264" s="8">
         <f>(D264*E264)</f>
@@ -42421,7 +42361,7 @@
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B265" s="8"/>
       <c r="C265" s="2">
@@ -42460,10 +42400,10 @@
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C267" s="8">
         <v>200</v>
@@ -42484,7 +42424,7 @@
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B268" s="8" t="s">
         <v>121</v>
@@ -42508,7 +42448,7 @@
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B269" s="8" t="s">
         <v>73</v>
@@ -42528,7 +42468,7 @@
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B270" s="8" t="s">
         <v>122</v>
@@ -42548,10 +42488,10 @@
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C271" s="8">
         <f>(D271*E271)</f>
@@ -42573,7 +42513,7 @@
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B272" s="8"/>
       <c r="C272" s="2">
@@ -42612,10 +42552,10 @@
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C274" s="8">
         <v>200</v>
@@ -42636,7 +42576,7 @@
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B275" s="8" t="s">
         <v>121</v>
@@ -42660,7 +42600,7 @@
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B276" s="8" t="s">
         <v>73</v>
@@ -42680,7 +42620,7 @@
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B277" s="8" t="s">
         <v>122</v>
@@ -42700,10 +42640,10 @@
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C278" s="8">
         <f>(D278*E278)</f>
@@ -42725,7 +42665,7 @@
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A279" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B279" s="8"/>
       <c r="C279" s="2">
@@ -42764,10 +42704,10 @@
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A281" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C281" s="8">
         <v>200</v>
@@ -42788,7 +42728,7 @@
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B282" s="8" t="s">
         <v>121</v>
@@ -42812,7 +42752,7 @@
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A283" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B283" s="8" t="s">
         <v>73</v>
@@ -42832,7 +42772,7 @@
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B284" s="8" t="s">
         <v>122</v>
@@ -42852,10 +42792,10 @@
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A285" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C285" s="8">
         <f>(D285*E285)</f>
@@ -42877,7 +42817,7 @@
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B286" s="8"/>
       <c r="C286" s="2">
@@ -42915,10 +42855,10 @@
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C288" s="8">
         <v>200</v>
@@ -42943,7 +42883,7 @@
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A289" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B289" s="8" t="s">
         <v>121</v>
@@ -42971,7 +42911,7 @@
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B290" s="8" t="s">
         <v>73</v>
@@ -42995,7 +42935,7 @@
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A291" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B291" s="8" t="s">
         <v>122</v>
@@ -43015,10 +42955,10 @@
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C292" s="8">
         <f>(D292*E292)</f>
@@ -43040,7 +42980,7 @@
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A293" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B293" s="8"/>
       <c r="C293" s="2">
@@ -43065,7 +43005,7 @@
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B294" s="8"/>
       <c r="C294" s="2"/>
@@ -43108,7 +43048,7 @@
         <v>176</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C296" s="8">
         <v>200</v>
@@ -43224,7 +43164,7 @@
         <v>176</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C301" s="8">
         <f>(D301*E301)</f>
@@ -43246,7 +43186,7 @@
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B302" s="8"/>
       <c r="C302" s="2">
@@ -43325,7 +43265,7 @@
     </row>
     <row r="306" spans="1:13" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B306" s="15"/>
       <c r="C306" s="13">
@@ -43487,7 +43427,7 @@
         <v>177</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C314" s="8">
         <f>(D314*E314)</f>
@@ -43509,7 +43449,7 @@
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A315" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B315" s="8"/>
       <c r="C315" s="2">
@@ -43647,7 +43587,7 @@
         <v>220</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C321" s="8">
         <f>(D321*E321)</f>
@@ -43669,7 +43609,7 @@
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B322" s="8"/>
       <c r="C322" s="2">
@@ -43784,7 +43724,7 @@
         <v>246</v>
       </c>
       <c r="B329" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C329">
         <f>(D329*E329)</f>
@@ -43799,7 +43739,7 @@
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C330" s="2">
         <f>SUM(C325:C329)</f>
@@ -43886,7 +43826,7 @@
         <v>250</v>
       </c>
       <c r="B336" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C336">
         <f>(D336*E336)</f>
@@ -43901,7 +43841,7 @@
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C337" s="2">
         <f>SUM(C332:C336)</f>
@@ -43956,7 +43896,7 @@
         <v>250</v>
       </c>
       <c r="G340" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H340">
         <v>2000</v>
@@ -43973,7 +43913,7 @@
         <v>250</v>
       </c>
       <c r="G341" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H341">
         <v>350</v>
@@ -44001,7 +43941,7 @@
         <v>254</v>
       </c>
       <c r="B343" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C343" s="8">
         <f>(D343*E343)</f>
@@ -44022,7 +43962,7 @@
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C344" s="2">
         <f>SUM(C339:C343)</f>
@@ -44051,7 +43991,7 @@
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B346" t="s">
         <v>73</v>
@@ -44068,7 +44008,7 @@
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B347" t="s">
         <v>122</v>
@@ -44085,7 +44025,7 @@
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B348" t="s">
         <v>234</v>
@@ -44102,7 +44042,7 @@
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B349" t="s">
         <v>236</v>
@@ -44113,10 +44053,10 @@
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B350" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C350">
         <f>(D350*E350)</f>
@@ -44131,7 +44071,7 @@
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C351" s="2">
         <f>SUM(C346:C350)</f>
@@ -44157,11 +44097,78 @@
       <c r="H352" s="35"/>
       <c r="I352" s="30"/>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A353" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B353" s="2"/>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A356" s="31"/>
+      <c r="B356" s="32"/>
+      <c r="C356" s="32"/>
+      <c r="D356" s="32"/>
+      <c r="E356" s="32"/>
+      <c r="F356" s="32"/>
+      <c r="G356" s="32"/>
+      <c r="H356" s="32"/>
+      <c r="I356" s="32"/>
+      <c r="J356" s="32"/>
+      <c r="K356" s="32"/>
+      <c r="L356" s="32"/>
+      <c r="M356" s="32"/>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A357" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B357" t="s">
+        <v>73</v>
+      </c>
+      <c r="C357">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A358" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B358" t="s">
+        <v>122</v>
+      </c>
+      <c r="C358">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A359" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B359" t="s">
+        <v>234</v>
+      </c>
+      <c r="C359">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A360" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B360" t="s">
+        <v>236</v>
+      </c>
+      <c r="C360">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A361" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B361" t="s">
+        <v>303</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44173,7 +44180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD1A8C-99DF-4166-8097-144C71FF7489}">
   <dimension ref="A1:BV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView topLeftCell="AK1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
   </sheetViews>
@@ -44197,99 +44204,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="26"/>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
       <c r="J1" s="27"/>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
       <c r="O1" s="25"/>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="50" t="s">
         <v>237</v>
       </c>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="U1" s="43" t="s">
-        <v>299</v>
-      </c>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Z1" s="45" t="s">
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="U1" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Z1" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AE1" s="40" t="s">
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AE1" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AJ1" s="51" t="s">
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AJ1" s="49" t="s">
         <v>240</v>
       </c>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
+      <c r="AM1" s="49"/>
       <c r="AO1" s="48" t="s">
         <v>241</v>
       </c>
       <c r="AP1" s="48"/>
       <c r="AQ1" s="48"/>
       <c r="AR1" s="48"/>
-      <c r="AT1" s="47" t="s">
+      <c r="AT1" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="AU1" s="47"/>
-      <c r="AV1" s="47"/>
-      <c r="AW1" s="47"/>
-      <c r="AY1" s="37" t="s">
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AY1" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="AZ1" s="37"/>
-      <c r="BA1" s="37"/>
-      <c r="BB1" s="37"/>
+      <c r="AZ1" s="40"/>
+      <c r="BA1" s="40"/>
+      <c r="BB1" s="40"/>
       <c r="BD1" s="48" t="s">
         <v>252</v>
       </c>
       <c r="BE1" s="48"/>
       <c r="BF1" s="48"/>
       <c r="BG1" s="48"/>
-      <c r="BI1" s="49" t="s">
-        <v>300</v>
-      </c>
-      <c r="BJ1" s="49"/>
-      <c r="BK1" s="49"/>
-      <c r="BL1" s="49"/>
-      <c r="BN1" s="50" t="s">
+      <c r="BI1" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="BJ1" s="47"/>
+      <c r="BK1" s="47"/>
+      <c r="BL1" s="47"/>
+      <c r="BN1" s="52" t="s">
         <v>253</v>
       </c>
-      <c r="BO1" s="50"/>
-      <c r="BP1" s="50"/>
-      <c r="BQ1" s="50"/>
-      <c r="BS1" s="46" t="s">
-        <v>315</v>
-      </c>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
+      <c r="BO1" s="52"/>
+      <c r="BP1" s="52"/>
+      <c r="BQ1" s="52"/>
+      <c r="BS1" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="BT1" s="50"/>
+      <c r="BU1" s="50"/>
+      <c r="BV1" s="50"/>
     </row>
     <row r="2" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -45012,6 +45019,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="BS1:BV1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="BI1:BL1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="AY1:BB1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="U1:X1"/>
@@ -45021,12 +45034,6 @@
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="P1:S1"/>
-    <mergeCell ref="BS1:BV1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="BD1:BG1"/>
-    <mergeCell ref="BI1:BL1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="AY1:BB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45037,7 +45044,7 @@
   <dimension ref="A1:AK101"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45066,21 +45073,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -45294,36 +45301,36 @@
     </row>
     <row r="11" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52" t="s">
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52" t="s">
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52" t="s">
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52" t="s">
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52" t="s">
+      <c r="U12" s="53"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="52"/>
+      <c r="X12" s="53"/>
+      <c r="Y12" s="53"/>
       <c r="Z12" s="23" t="s">
         <v>82</v>
       </c>
@@ -45606,51 +45613,51 @@
     </row>
     <row r="23" spans="1:37" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="53" t="s">
+      <c r="H24" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53" t="s">
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53" t="s">
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53" t="s">
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53" t="s">
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
+      <c r="T24" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="U24" s="53"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="53" t="s">
+      <c r="U24" s="54"/>
+      <c r="V24" s="54"/>
+      <c r="W24" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="X24" s="53"/>
-      <c r="Y24" s="53"/>
-      <c r="Z24" s="53" t="s">
+      <c r="X24" s="54"/>
+      <c r="Y24" s="54"/>
+      <c r="Z24" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="AA24" s="53"/>
-      <c r="AB24" s="53"/>
-      <c r="AC24" s="53" t="s">
+      <c r="AA24" s="54"/>
+      <c r="AB24" s="54"/>
+      <c r="AC24" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="AD24" s="53"/>
-      <c r="AE24" s="53"/>
-      <c r="AF24" s="53" t="s">
+      <c r="AD24" s="54"/>
+      <c r="AE24" s="54"/>
+      <c r="AF24" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="AG24" s="53"/>
-      <c r="AH24" s="53"/>
+      <c r="AG24" s="54"/>
+      <c r="AH24" s="54"/>
     </row>
     <row r="25" spans="1:37" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H25" s="13" t="s">
@@ -45995,36 +46002,36 @@
     </row>
     <row r="35" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H36" s="53" t="s">
+      <c r="H36" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53" t="s">
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53" t="s">
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53" t="s">
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="53" t="s">
+      <c r="R36" s="54"/>
+      <c r="S36" s="54"/>
+      <c r="T36" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="U36" s="53"/>
-      <c r="V36" s="53"/>
-      <c r="W36" s="53" t="s">
+      <c r="U36" s="54"/>
+      <c r="V36" s="54"/>
+      <c r="W36" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="X36" s="53"/>
-      <c r="Y36" s="53"/>
+      <c r="X36" s="54"/>
+      <c r="Y36" s="54"/>
     </row>
     <row r="37" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H37" s="13" t="s">
@@ -46305,16 +46312,16 @@
     </row>
     <row r="47" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H48" s="52" t="s">
+      <c r="H48" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="52" t="s">
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
     </row>
     <row r="49" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H49" s="2" t="s">
@@ -46538,21 +46545,21 @@
     </row>
     <row r="59" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H60" s="53" t="s">
+      <c r="H60" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="53" t="s">
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+      <c r="K60" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="L60" s="53"/>
-      <c r="M60" s="53"/>
-      <c r="N60" s="53" t="s">
+      <c r="L60" s="54"/>
+      <c r="M60" s="54"/>
+      <c r="N60" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="O60" s="53"/>
-      <c r="P60" s="53"/>
+      <c r="O60" s="54"/>
+      <c r="P60" s="54"/>
     </row>
     <row r="61" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H61" s="2" t="s">
@@ -46791,21 +46798,21 @@
     </row>
     <row r="71" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="H72" s="52" t="s">
+      <c r="H72" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="I72" s="52"/>
-      <c r="J72" s="52"/>
-      <c r="K72" s="52" t="s">
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="L72" s="52"/>
-      <c r="M72" s="52"/>
-      <c r="N72" s="52" t="s">
+      <c r="L72" s="53"/>
+      <c r="M72" s="53"/>
+      <c r="N72" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="O72" s="52"/>
-      <c r="P72" s="52"/>
+      <c r="O72" s="53"/>
+      <c r="P72" s="53"/>
     </row>
     <row r="73" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H73" s="2" t="s">
@@ -47138,26 +47145,26 @@
     </row>
     <row r="83" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="84" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H84" s="52" t="s">
+      <c r="H84" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="I84" s="52"/>
-      <c r="J84" s="52"/>
-      <c r="K84" s="52" t="s">
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="L84" s="52"/>
-      <c r="M84" s="52"/>
-      <c r="N84" s="52" t="s">
+      <c r="L84" s="53"/>
+      <c r="M84" s="53"/>
+      <c r="N84" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="O84" s="52"/>
-      <c r="P84" s="52"/>
-      <c r="Q84" s="52" t="s">
+      <c r="O84" s="53"/>
+      <c r="P84" s="53"/>
+      <c r="Q84" s="53" t="s">
         <v>227</v>
       </c>
-      <c r="R84" s="52"/>
-      <c r="S84" s="52"/>
+      <c r="R84" s="53"/>
+      <c r="S84" s="53"/>
     </row>
     <row r="85" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H85" s="2" t="s">
@@ -47441,16 +47448,16 @@
     </row>
     <row r="95" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="96" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="H96" s="52" t="s">
+      <c r="H96" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="I96" s="52"/>
-      <c r="J96" s="52"/>
-      <c r="K96" s="52" t="s">
+      <c r="I96" s="53"/>
+      <c r="J96" s="53"/>
+      <c r="K96" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="L96" s="52"/>
-      <c r="M96" s="52"/>
+      <c r="L96" s="53"/>
+      <c r="M96" s="53"/>
     </row>
     <row r="97" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H97" s="2" t="s">
@@ -47537,7 +47544,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B101">
         <v>2129</v>
@@ -47551,12 +47558,36 @@
       <c r="E101">
         <v>76029.149999999994</v>
       </c>
+      <c r="H101">
+        <v>1236</v>
+      </c>
       <c r="K101">
         <v>893</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="H96:J96"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="Z24:AB24"/>
+    <mergeCell ref="AC24:AE24"/>
+    <mergeCell ref="AF24:AH24"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="T36:V36"/>
+    <mergeCell ref="W36:Y36"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
     <mergeCell ref="H84:J84"/>
     <mergeCell ref="K84:M84"/>
     <mergeCell ref="Q12:S12"/>
@@ -47573,27 +47604,6 @@
     <mergeCell ref="N60:P60"/>
     <mergeCell ref="N84:P84"/>
     <mergeCell ref="Q84:S84"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="H96:J96"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="Z24:AB24"/>
-    <mergeCell ref="AC24:AE24"/>
-    <mergeCell ref="AF24:AH24"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="Q36:S36"/>
-    <mergeCell ref="T36:V36"/>
-    <mergeCell ref="W36:Y36"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -47605,8 +47615,8 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47685,10 +47695,10 @@
         <v>44385</v>
       </c>
       <c r="B3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" t="s">
         <v>319</v>
-      </c>
-      <c r="C3" t="s">
-        <v>320</v>
       </c>
       <c r="D3">
         <v>714</v>
@@ -47835,12 +47845,9 @@
         <f t="shared" ref="H10:H16" si="2">(F10)</f>
         <v>2357.0500000000002</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
         <v>-2932.0999999999995</v>
-      </c>
-      <c r="K10" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -48086,7 +48093,7 @@
         <v>44394</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D21">
         <v>714</v>
@@ -48112,7 +48119,7 @@
         <v>44394</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D22">
         <v>510</v>
@@ -48164,7 +48171,7 @@
         <v>44395</v>
       </c>
       <c r="B24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D24">
         <v>561</v>
@@ -48190,7 +48197,7 @@
         <v>44395</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D25">
         <v>910</v>
@@ -48242,7 +48249,7 @@
         <v>44398</v>
       </c>
       <c r="B27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D27">
         <v>680</v>
@@ -48268,7 +48275,7 @@
         <v>44398</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D28">
         <v>425</v>
@@ -48320,7 +48327,7 @@
         <v>44398</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D30">
         <v>731</v>
@@ -48346,7 +48353,7 @@
         <v>44398</v>
       </c>
       <c r="B31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D31">
         <v>561</v>
@@ -48372,7 +48379,7 @@
         <v>44398</v>
       </c>
       <c r="B32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D32">
         <v>306</v>
@@ -48398,7 +48405,7 @@
         <v>44398</v>
       </c>
       <c r="B33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D33">
         <v>408</v>
@@ -48424,7 +48431,7 @@
         <v>44398</v>
       </c>
       <c r="B34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D34">
         <v>1156</v>
@@ -48450,10 +48457,10 @@
         <v>44399</v>
       </c>
       <c r="B35" t="s">
+        <v>318</v>
+      </c>
+      <c r="C35" t="s">
         <v>319</v>
-      </c>
-      <c r="C35" t="s">
-        <v>320</v>
       </c>
       <c r="D35">
         <v>510</v>
@@ -48479,7 +48486,7 @@
         <v>44399</v>
       </c>
       <c r="B36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D36">
         <v>204</v>
@@ -48502,13 +48509,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37" t="s">
         <v>280</v>
       </c>
-      <c r="B37" t="s">
-        <v>281</v>
-      </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D37">
         <v>340</v>
@@ -48534,10 +48541,10 @@
         <v>44399</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D38">
         <v>85</v>
@@ -48563,10 +48570,10 @@
         <v>44399</v>
       </c>
       <c r="B39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D39">
         <v>221</v>
@@ -48618,10 +48625,10 @@
         <v>44399</v>
       </c>
       <c r="B41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C41" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D41">
         <v>408</v>
@@ -48647,7 +48654,7 @@
         <v>44399</v>
       </c>
       <c r="B42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D42">
         <v>748</v>
@@ -48673,7 +48680,7 @@
         <v>44399</v>
       </c>
       <c r="B43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D43">
         <v>629</v>
@@ -48699,7 +48706,7 @@
         <v>44399</v>
       </c>
       <c r="B44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D44">
         <v>799</v>
@@ -48725,10 +48732,10 @@
         <v>44400</v>
       </c>
       <c r="B45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D45">
         <v>255</v>
@@ -48754,7 +48761,7 @@
         <v>44400</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C46" t="s">
         <v>223</v>
@@ -48783,10 +48790,10 @@
         <v>44400</v>
       </c>
       <c r="B47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D47">
         <v>748</v>
@@ -48819,7 +48826,7 @@
         <v>12067.750000000004</v>
       </c>
       <c r="K48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
@@ -48827,10 +48834,10 @@
         <v>44401</v>
       </c>
       <c r="B49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D49">
         <v>408</v>
@@ -48856,7 +48863,7 @@
         <v>44401</v>
       </c>
       <c r="B50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D50">
         <v>459</v>
@@ -48882,10 +48889,10 @@
         <v>44401</v>
       </c>
       <c r="B51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D51">
         <v>799</v>
@@ -48911,7 +48918,7 @@
         <v>44401</v>
       </c>
       <c r="B52" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D52">
         <v>1020</v>
@@ -48937,7 +48944,7 @@
         <v>44402</v>
       </c>
       <c r="B53" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D53">
         <v>119</v>
@@ -48963,10 +48970,10 @@
         <v>44402</v>
       </c>
       <c r="B54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D54">
         <v>272</v>
@@ -49018,10 +49025,10 @@
         <v>44402</v>
       </c>
       <c r="B56" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D56">
         <v>714</v>
@@ -49047,7 +49054,7 @@
         <v>44402</v>
       </c>
       <c r="B57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D57">
         <v>901</v>
@@ -49073,7 +49080,7 @@
         <v>44402</v>
       </c>
       <c r="B58" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D58">
         <v>204</v>
@@ -49106,7 +49113,7 @@
         <v>-16533.449999999993</v>
       </c>
       <c r="K59" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 ve 3 ağustos işlendi
</commit_message>
<xml_diff>
--- a/Muhasebe.xlsx
+++ b/Muhasebe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BELEVİ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FCBEF8-6957-432D-95EE-724C220561CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EBA661-84CF-4764-B04F-DF229F3B89F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" activeTab="3" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10640" activeTab="2" xr2:uid="{B38A589B-49D3-4226-8883-CE6CE99F1FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GÜNLÜK_GELEN_GİDEN_MAL" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="319">
   <si>
     <t>MÜSTAHSİL</t>
   </si>
@@ -765,9 +765,6 @@
     <t>ŞABAN OK</t>
   </si>
   <si>
-    <t>SERCAN GÜR</t>
-  </si>
-  <si>
     <t>YUSUF AKINCI</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
   </si>
   <si>
     <t>Sıtkı Adsız</t>
-  </si>
-  <si>
-    <t>CEMAL ŞİMŞEK</t>
   </si>
   <si>
     <t>SALİH ELDEN</t>
@@ -936,9 +930,6 @@
     <t>FERİT _ADSIZ</t>
   </si>
   <si>
-    <t>HALİL AĞIR</t>
-  </si>
-  <si>
     <t>Ali Yücel</t>
   </si>
   <si>
@@ -1002,9 +993,6 @@
     <t>AYSU_GIDA</t>
   </si>
   <si>
-    <t>ÇÜRÜK</t>
-  </si>
-  <si>
     <t>ÇEK(40)</t>
   </si>
   <si>
@@ -1012,6 +1000,9 @@
   </si>
   <si>
     <t>2.8.2021/PAZARTESİ</t>
+  </si>
+  <si>
+    <t>3.8.2021/SALI</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1028,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,12 +1056,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1165,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1177,8 +1162,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,9 +1173,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -1201,7 +1186,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1209,23 +1194,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1235,25 +1220,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1271,22 +1256,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1603,13 +1585,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39BD046-FBF6-4454-99AD-0B843F600705}">
-  <dimension ref="A1:BU515"/>
+  <dimension ref="A1:BU524"/>
   <sheetViews>
     <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="BB500" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="BT521" sqref="BT521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1764,7 +1746,7 @@
       <c r="BN1" s="49"/>
       <c r="BO1" s="49"/>
       <c r="BP1" s="46" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BQ1" s="46"/>
       <c r="BR1" s="46"/>
@@ -2160,7 +2142,7 @@
         <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I5">
         <v>3500.85</v>
@@ -2642,7 +2624,7 @@
         <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I11">
         <v>3014.4</v>
@@ -3300,7 +3282,7 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I19">
         <v>3909.75</v>
@@ -4171,7 +4153,7 @@
         <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4774,7 +4756,7 @@
         <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -5847,7 +5829,7 @@
         <v>138</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -6849,7 +6831,7 @@
         <v>142</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -7863,7 +7845,7 @@
         <v>145</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -9150,7 +9132,7 @@
         <v>149</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -10258,7 +10240,7 @@
         <v>153</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
@@ -11157,7 +11139,7 @@
         <v>156</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="15"/>
@@ -12055,7 +12037,7 @@
         <v>158</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
@@ -12968,7 +12950,7 @@
         <v>160</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -13781,7 +13763,7 @@
         <v>162</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
@@ -14590,7 +14572,7 @@
         <v>163</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
@@ -15594,7 +15576,7 @@
         <v>165</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
@@ -16976,7 +16958,7 @@
         <v>167</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
@@ -18081,7 +18063,7 @@
         <v>169</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
@@ -18993,7 +18975,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="8"/>
@@ -20100,7 +20082,7 @@
         <v>171</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C204" s="8"/>
       <c r="D204" s="8"/>
@@ -21003,7 +20985,7 @@
         <v>175</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C214" s="8"/>
       <c r="D214" s="8"/>
@@ -21808,7 +21790,7 @@
         <v>180</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C223" s="8"/>
       <c r="D223" s="8"/>
@@ -22518,7 +22500,7 @@
         <v>181</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C231" s="8"/>
       <c r="D231" s="8"/>
@@ -23417,7 +23399,7 @@
         <v>183</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C241" s="8"/>
       <c r="D241" s="8"/>
@@ -24223,7 +24205,7 @@
         <v>185</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C250" s="8"/>
       <c r="D250" s="8"/>
@@ -25311,7 +25293,7 @@
         <v>186</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C262" s="8"/>
       <c r="D262" s="8"/>
@@ -26023,7 +26005,7 @@
         <v>187</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C270" s="8"/>
       <c r="D270" s="8"/>
@@ -26735,7 +26717,7 @@
         <v>188</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C278" s="8"/>
       <c r="D278" s="8"/>
@@ -26969,7 +26951,9 @@
       <c r="BC280" s="2"/>
       <c r="BD280" s="11"/>
       <c r="BE280" s="11"/>
-      <c r="BF280" s="11"/>
+      <c r="BF280">
+        <v>460</v>
+      </c>
       <c r="BG280" s="11"/>
       <c r="BH280" s="11"/>
       <c r="BI280" s="11"/>
@@ -27353,7 +27337,7 @@
         <v>190</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C285" s="8"/>
       <c r="D285" s="8"/>
@@ -28440,7 +28424,7 @@
         <v>191</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C297" s="8"/>
       <c r="D297" s="8"/>
@@ -29154,7 +29138,7 @@
         <v>192</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C305" s="8"/>
       <c r="D305" s="8"/>
@@ -30060,7 +30044,7 @@
         <v>193</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C315" s="8"/>
       <c r="D315" s="8"/>
@@ -30873,7 +30857,7 @@
         <v>194</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C324" s="8"/>
       <c r="D324" s="8"/>
@@ -32077,7 +32061,7 @@
         <v>195</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C337" s="8"/>
       <c r="D337" s="8"/>
@@ -32987,7 +32971,7 @@
         <v>199</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C347" s="8"/>
       <c r="D347" s="8"/>
@@ -33732,7 +33716,7 @@
         <v>19</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I360">
         <v>8774.25</v>
@@ -34137,7 +34121,7 @@
         <v>20</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I368">
         <v>7451.2</v>
@@ -34582,7 +34566,7 @@
         <v>24</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I378">
         <v>10113.75</v>
@@ -34951,7 +34935,7 @@
         <v>27</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I386">
         <v>5961.3</v>
@@ -35296,7 +35280,7 @@
         <v>29</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I396">
         <v>9131.4500000000007</v>
@@ -35681,7 +35665,7 @@
         <v>38</v>
       </c>
       <c r="B408" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I408" s="7">
         <v>8358.2999999999993</v>
@@ -36094,7 +36078,7 @@
         <v>90</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I422">
         <v>19524.7</v>
@@ -36591,7 +36575,7 @@
         <v>177</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I439">
         <v>19217.349999999999</v>
@@ -36836,7 +36820,7 @@
         <v>220</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I450">
         <v>11786.95</v>
@@ -36882,10 +36866,10 @@
     </row>
     <row r="455" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A455" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B455" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D455">
         <v>486</v>
@@ -36916,10 +36900,10 @@
     </row>
     <row r="456" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A456" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B456" t="s">
         <v>245</v>
-      </c>
-      <c r="B456" t="s">
-        <v>246</v>
       </c>
       <c r="D456">
         <v>48</v>
@@ -36944,7 +36928,7 @@
     </row>
     <row r="457" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A457" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B457" t="s">
         <v>14</v>
@@ -36972,10 +36956,10 @@
     </row>
     <row r="458" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A458" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B458" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D458">
         <v>759</v>
@@ -37000,7 +36984,7 @@
     </row>
     <row r="459" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A459" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B459" t="s">
         <v>117</v>
@@ -37028,7 +37012,7 @@
     </row>
     <row r="460" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A460" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B460" t="s">
         <v>117</v>
@@ -37056,7 +37040,7 @@
     </row>
     <row r="461" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A461" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B461" t="s">
         <v>8</v>
@@ -37084,10 +37068,10 @@
     </row>
     <row r="462" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A462" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B462" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H462" s="6"/>
       <c r="I462">
@@ -37144,7 +37128,7 @@
     </row>
     <row r="466" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A466" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B466" t="s">
         <v>140</v>
@@ -37187,7 +37171,7 @@
     </row>
     <row r="467" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A467" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B467" t="s">
         <v>28</v>
@@ -37230,7 +37214,7 @@
     </row>
     <row r="468" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A468" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B468" t="s">
         <v>8</v>
@@ -37262,7 +37246,7 @@
     </row>
     <row r="469" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A469" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B469" t="s">
         <v>26</v>
@@ -37293,7 +37277,7 @@
     </row>
     <row r="470" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A470" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B470" t="s">
         <v>117</v>
@@ -37324,7 +37308,7 @@
     </row>
     <row r="471" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A471" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B471" t="s">
         <v>217</v>
@@ -37355,10 +37339,10 @@
     </row>
     <row r="472" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A472" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B472" t="s">
         <v>248</v>
-      </c>
-      <c r="B472" t="s">
-        <v>249</v>
       </c>
       <c r="C472" t="s">
         <v>9</v>
@@ -37386,10 +37370,10 @@
     </row>
     <row r="473" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A473" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B473" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C473" t="s">
         <v>9</v>
@@ -37417,7 +37401,7 @@
     </row>
     <row r="474" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A474" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B474" t="s">
         <v>14</v>
@@ -37448,7 +37432,7 @@
     </row>
     <row r="475" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A475" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B475" t="s">
         <v>22</v>
@@ -37479,7 +37463,7 @@
     </row>
     <row r="476" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A476" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B476" t="s">
         <v>15</v>
@@ -37510,7 +37494,7 @@
     </row>
     <row r="477" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A477" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B477" t="s">
         <v>15</v>
@@ -37541,10 +37525,10 @@
     </row>
     <row r="478" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A478" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B478" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I478">
         <v>13790.3</v>
@@ -37583,7 +37567,7 @@
         <f>SUM(BH466:BH477)</f>
         <v>3072</v>
       </c>
-      <c r="BT479">
+      <c r="BT479" s="2">
         <f>(BD479+BH479)</f>
         <v>4698</v>
       </c>
@@ -37597,9 +37581,9 @@
         <v>7.441087184006169</v>
       </c>
     </row>
-    <row r="482" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A482" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B482" t="s">
         <v>22</v>
@@ -37628,9 +37612,9 @@
         <v>10743.9</v>
       </c>
     </row>
-    <row r="483" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A483" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B483" t="s">
         <v>8</v>
@@ -37659,9 +37643,9 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="484" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A484" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B484" t="s">
         <v>31</v>
@@ -37690,12 +37674,12 @@
         <v>20300</v>
       </c>
     </row>
-    <row r="485" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A485" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B485" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C485" t="s">
         <v>9</v>
@@ -37721,9 +37705,9 @@
         <v>9200</v>
       </c>
     </row>
-    <row r="486" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A486" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B486" t="s">
         <v>26</v>
@@ -37752,9 +37736,9 @@
         <v>29032</v>
       </c>
     </row>
-    <row r="487" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A487" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B487" t="s">
         <v>215</v>
@@ -37783,9 +37767,9 @@
         <v>18860.399999999998</v>
       </c>
     </row>
-    <row r="488" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A488" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B488" t="s">
         <v>28</v>
@@ -37814,9 +37798,9 @@
         <v>13392</v>
       </c>
     </row>
-    <row r="489" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A489" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B489" t="s">
         <v>15</v>
@@ -37845,18 +37829,18 @@
         <v>18039</v>
       </c>
     </row>
-    <row r="490" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A490" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B490" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I490">
         <v>17450</v>
       </c>
     </row>
-    <row r="491" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B491" s="2" t="s">
         <v>17</v>
       </c>
@@ -37881,7 +37865,7 @@
         <v>138085.29999999999</v>
       </c>
     </row>
-    <row r="492" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B492" s="2" t="s">
         <v>18</v>
       </c>
@@ -37890,10 +37874,10 @@
         <v>8.0685579058081096</v>
       </c>
     </row>
-    <row r="493" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="494" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="494" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A494" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B494" t="s">
         <v>8</v>
@@ -37927,10 +37911,14 @@
       <c r="BH494">
         <v>893</v>
       </c>
-    </row>
-    <row r="495" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="BT494" s="2">
+        <f>(BD494+BH494)</f>
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="495" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A495" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B495" s="8" t="s">
         <v>14</v>
@@ -37959,9 +37947,9 @@
         <v>20724</v>
       </c>
     </row>
-    <row r="496" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A496" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B496" s="8" t="s">
         <v>15</v>
@@ -37990,9 +37978,9 @@
         <v>21750</v>
       </c>
     </row>
-    <row r="497" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A497" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B497" s="8" t="s">
         <v>26</v>
@@ -38021,18 +38009,18 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="498" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="498" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A498" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B498" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I498" s="14">
         <v>8253.15</v>
       </c>
     </row>
-    <row r="499" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="499" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B499" s="2" t="s">
         <v>17</v>
       </c>
@@ -38058,7 +38046,7 @@
         <v>76029.149999999994</v>
       </c>
     </row>
-    <row r="500" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="500" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B500" s="2" t="s">
         <v>18</v>
       </c>
@@ -38067,9 +38055,9 @@
         <v>7.465548900235663</v>
       </c>
     </row>
-    <row r="502" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="502" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A502" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B502" t="s">
         <v>14</v>
@@ -38098,18 +38086,18 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="503" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A503" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B503" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I503">
         <v>1329</v>
       </c>
     </row>
-    <row r="504" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="504" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B504" s="2" t="s">
         <v>17</v>
       </c>
@@ -38130,7 +38118,7 @@
         <v>3889</v>
       </c>
     </row>
-    <row r="505" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="505" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B505" s="2" t="s">
         <v>18</v>
       </c>
@@ -38139,12 +38127,12 @@
         <v>6.0765624999999996</v>
       </c>
     </row>
-    <row r="506" spans="1:68" s="31" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:72" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A506" s="30"/>
     </row>
-    <row r="507" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A507" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B507" t="s">
         <v>14</v>
@@ -38181,13 +38169,17 @@
       <c r="BP507">
         <v>274</v>
       </c>
-    </row>
-    <row r="508" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="BT507">
+        <f>(BD507+BH507+BP507)</f>
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="508" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A508" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B508" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C508" t="s">
         <v>9</v>
@@ -38213,9 +38205,9 @@
         <v>13986.699999999999</v>
       </c>
     </row>
-    <row r="509" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A509" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B509" t="s">
         <v>26</v>
@@ -38244,9 +38236,9 @@
         <v>26364</v>
       </c>
     </row>
-    <row r="510" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="510" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A510" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B510" t="s">
         <v>215</v>
@@ -38275,19 +38267,19 @@
         <v>9318.5499999999993</v>
       </c>
     </row>
-    <row r="511" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A511" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B511" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D511" s="2"/>
       <c r="I511">
         <v>7212</v>
       </c>
     </row>
-    <row r="512" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B512" s="2" t="s">
         <v>17</v>
       </c>
@@ -38313,7 +38305,7 @@
         <v>64959.25</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="513" spans="1:72" x14ac:dyDescent="0.35">
       <c r="B513" s="2" t="s">
         <v>18</v>
       </c>
@@ -38322,9 +38314,201 @@
         <v>7.2620737842370042</v>
       </c>
     </row>
-    <row r="515" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="515" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A515" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
+      </c>
+      <c r="B515" t="s">
+        <v>15</v>
+      </c>
+      <c r="D515">
+        <v>860</v>
+      </c>
+      <c r="E515">
+        <v>3460</v>
+      </c>
+      <c r="F515">
+        <v>345</v>
+      </c>
+      <c r="G515">
+        <f>(E515-F515)</f>
+        <v>3115</v>
+      </c>
+      <c r="H515">
+        <v>7</v>
+      </c>
+      <c r="I515">
+        <f>(G515*H515)</f>
+        <v>21805</v>
+      </c>
+      <c r="BH515">
+        <v>460</v>
+      </c>
+      <c r="BP515">
+        <v>400</v>
+      </c>
+      <c r="BT515">
+        <f>(BH515+BP515)</f>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="516" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A516" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B516" t="s">
+        <v>299</v>
+      </c>
+      <c r="I516">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="517" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="B517" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D517" s="2">
+        <f t="shared" ref="D517:I517" si="116">SUM(D515:D516)</f>
+        <v>860</v>
+      </c>
+      <c r="E517" s="2">
+        <f t="shared" si="116"/>
+        <v>3460</v>
+      </c>
+      <c r="F517" s="2">
+        <f t="shared" si="116"/>
+        <v>345</v>
+      </c>
+      <c r="G517" s="2">
+        <f t="shared" si="116"/>
+        <v>3115</v>
+      </c>
+      <c r="H517" s="2"/>
+      <c r="I517" s="2">
+        <f t="shared" si="116"/>
+        <v>24826</v>
+      </c>
+    </row>
+    <row r="518" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="B518" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H518" s="2">
+        <f>(I517/G517)</f>
+        <v>7.9698234349919739</v>
+      </c>
+    </row>
+    <row r="520" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A520" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B520" t="s">
+        <v>15</v>
+      </c>
+      <c r="D520">
+        <v>398</v>
+      </c>
+      <c r="E520">
+        <v>1760</v>
+      </c>
+      <c r="F520">
+        <v>175</v>
+      </c>
+      <c r="G520">
+        <f>(E520-F520)</f>
+        <v>1585</v>
+      </c>
+      <c r="H520">
+        <v>7</v>
+      </c>
+      <c r="I520">
+        <f>(G520*H520)</f>
+        <v>11095</v>
+      </c>
+      <c r="BH520">
+        <v>504</v>
+      </c>
+      <c r="BP520">
+        <v>400</v>
+      </c>
+      <c r="BT520">
+        <f>(BH520+BP520)</f>
+        <v>904</v>
+      </c>
+    </row>
+    <row r="521" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A521" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B521" t="s">
+        <v>26</v>
+      </c>
+      <c r="D521">
+        <v>506</v>
+      </c>
+      <c r="E521">
+        <v>1920</v>
+      </c>
+      <c r="F521">
+        <v>220</v>
+      </c>
+      <c r="G521">
+        <f>(E521-F521)</f>
+        <v>1700</v>
+      </c>
+      <c r="H521">
+        <v>7</v>
+      </c>
+      <c r="I521">
+        <f>(G521*H521)</f>
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="522" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A522" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B522" t="s">
+        <v>299</v>
+      </c>
+      <c r="D522" s="2"/>
+      <c r="I522">
+        <v>3124.4</v>
+      </c>
+    </row>
+    <row r="523" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="B523" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D523" s="2">
+        <f t="shared" ref="D523:I523" si="117">SUM(D520:D522)</f>
+        <v>904</v>
+      </c>
+      <c r="E523" s="2">
+        <f t="shared" si="117"/>
+        <v>3680</v>
+      </c>
+      <c r="F523" s="2">
+        <f t="shared" si="117"/>
+        <v>395</v>
+      </c>
+      <c r="G523" s="2">
+        <f t="shared" si="117"/>
+        <v>3285</v>
+      </c>
+      <c r="H523" s="2"/>
+      <c r="I523" s="2">
+        <f t="shared" si="117"/>
+        <v>26119.4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="B524" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H524" s="2">
+        <f>(I523/G523)</f>
+        <v>7.9511111111111115</v>
       </c>
     </row>
   </sheetData>
@@ -38352,10 +38536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F781AA57-6247-4A4F-9752-70CC607DC978}">
-  <dimension ref="A1:AK110"/>
+  <dimension ref="A1:AK111"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A88" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39689,7 +39873,7 @@
         <v>12005</v>
       </c>
       <c r="E50" s="6">
-        <v>66336.25</v>
+        <v>77704.899999999994</v>
       </c>
       <c r="F50" s="40"/>
       <c r="H50">
@@ -39713,7 +39897,7 @@
         <v>6568</v>
       </c>
       <c r="E51" s="6">
-        <v>37760</v>
+        <v>44546.15</v>
       </c>
       <c r="F51" s="40"/>
       <c r="H51">
@@ -39737,7 +39921,7 @@
         <v>10342</v>
       </c>
       <c r="E52" s="6">
-        <v>57291</v>
+        <v>66596.350000000006</v>
       </c>
       <c r="F52" s="40"/>
       <c r="H52">
@@ -39761,7 +39945,7 @@
         <v>6463</v>
       </c>
       <c r="E53" s="6">
-        <v>39774.5</v>
+        <v>46372.65</v>
       </c>
       <c r="F53" s="40"/>
       <c r="H53">
@@ -39785,7 +39969,7 @@
         <v>8479</v>
       </c>
       <c r="E54" s="6">
-        <v>51469.5</v>
+        <v>59785.5</v>
       </c>
       <c r="F54" s="40"/>
       <c r="H54">
@@ -39809,7 +39993,7 @@
         <v>2690</v>
       </c>
       <c r="E55" s="6">
-        <v>14086</v>
+        <v>18505.7</v>
       </c>
       <c r="F55" s="40"/>
       <c r="H55">
@@ -39837,7 +40021,7 @@
       </c>
       <c r="E56" s="2">
         <f t="shared" si="4"/>
-        <v>266717.25</v>
+        <v>313511.25</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" t="s">
@@ -39939,7 +40123,7 @@
         <v>13449</v>
       </c>
       <c r="E62" s="6">
-        <v>92809.5</v>
+        <v>104598.8</v>
       </c>
       <c r="F62" s="40"/>
       <c r="H62">
@@ -39963,7 +40147,7 @@
         <v>7972</v>
       </c>
       <c r="E63" s="6">
-        <v>53028.600000000006</v>
+        <v>60954.5</v>
       </c>
       <c r="F63" s="40"/>
       <c r="H63">
@@ -39987,7 +40171,7 @@
         <v>8442</v>
       </c>
       <c r="E64" s="6">
-        <v>58727.5</v>
+        <v>66500.649999999994</v>
       </c>
       <c r="F64" s="40"/>
       <c r="H64">
@@ -40011,7 +40195,7 @@
         <v>10341</v>
       </c>
       <c r="E65" s="6">
-        <v>57998.25</v>
+        <v>67298.899999999994</v>
       </c>
       <c r="F65" s="40"/>
       <c r="H65">
@@ -40038,7 +40222,7 @@
         <v>13276</v>
       </c>
       <c r="E66" s="6">
-        <v>80914</v>
+        <v>90929.05</v>
       </c>
       <c r="F66" s="40"/>
       <c r="H66">
@@ -40062,7 +40246,7 @@
         <v>4875</v>
       </c>
       <c r="E67" s="6">
-        <v>29387</v>
+        <v>34631.550000000003</v>
       </c>
       <c r="F67" s="40"/>
       <c r="H67">
@@ -40090,7 +40274,7 @@
       </c>
       <c r="E68" s="2">
         <f t="shared" si="5"/>
-        <v>372864.85</v>
+        <v>424913.44999999995</v>
       </c>
       <c r="F68" s="13"/>
       <c r="G68" t="s">
@@ -40195,7 +40379,7 @@
         <v>9762</v>
       </c>
       <c r="E74" s="6">
-        <v>63851.5</v>
+        <v>72625.75</v>
       </c>
       <c r="F74" s="40"/>
       <c r="H74" s="6">
@@ -40224,7 +40408,7 @@
         <v>7750</v>
       </c>
       <c r="E75" s="6">
-        <v>48226.5</v>
+        <v>55677.7</v>
       </c>
       <c r="F75" s="40"/>
       <c r="H75" s="6">
@@ -40253,7 +40437,7 @@
         <v>12631</v>
       </c>
       <c r="E76" s="6">
-        <v>84508.3</v>
+        <v>94622.05</v>
       </c>
       <c r="F76" s="40"/>
       <c r="H76" s="6">
@@ -40282,7 +40466,7 @@
         <v>4465</v>
       </c>
       <c r="E77" s="6">
-        <v>27477.5</v>
+        <v>33438.800000000003</v>
       </c>
       <c r="F77" s="40"/>
       <c r="H77" s="6">
@@ -40308,7 +40492,7 @@
         <v>10276</v>
       </c>
       <c r="E78" s="6">
-        <v>64623.15</v>
+        <v>73754.600000000006</v>
       </c>
       <c r="F78" s="40"/>
       <c r="H78" s="6">
@@ -40337,7 +40521,7 @@
         <v>9216</v>
       </c>
       <c r="E79" s="6">
-        <v>56907.65</v>
+        <v>65265.95</v>
       </c>
       <c r="F79" s="40"/>
       <c r="H79" s="6">
@@ -40370,7 +40554,7 @@
       </c>
       <c r="E80" s="2">
         <f t="shared" si="6"/>
-        <v>345594.60000000003</v>
+        <v>395384.85000000003</v>
       </c>
       <c r="F80" s="13"/>
       <c r="G80" t="s">
@@ -40560,7 +40744,7 @@
         <v>24238</v>
       </c>
       <c r="E86">
-        <v>164057.1</v>
+        <v>183581.8</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.35">
@@ -40577,7 +40761,7 @@
         <v>25004</v>
       </c>
       <c r="E87">
-        <v>195360</v>
+        <v>222687.4</v>
       </c>
       <c r="N87">
         <v>648</v>
@@ -40698,11 +40882,11 @@
       </c>
       <c r="E93" s="2">
         <f>SUM(E86:E89)</f>
-        <v>457453.39999999997</v>
+        <v>504305.49999999994</v>
       </c>
       <c r="F93" s="13">
         <f>(E93/D93)</f>
-        <v>7.2236707881314439</v>
+        <v>7.9635147725298836</v>
       </c>
       <c r="H93" s="2">
         <v>4897</v>
@@ -40821,7 +41005,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B98">
         <v>2427</v>
@@ -40844,7 +41028,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B99">
         <v>4698</v>
@@ -40867,7 +41051,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B100">
         <v>4057</v>
@@ -40879,12 +41063,12 @@
         <v>14537</v>
       </c>
       <c r="E100">
-        <v>102596.3</v>
+        <v>138085.29999999999</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B101">
         <v>2129</v>
@@ -40907,7 +41091,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B102">
         <v>140</v>
@@ -40940,7 +41124,7 @@
       </c>
       <c r="E103" s="2">
         <f t="shared" si="9"/>
-        <v>388932.54999999993</v>
+        <v>424421.54999999993</v>
       </c>
     </row>
     <row r="106" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.35">
@@ -40958,7 +41142,7 @@
       <c r="L107" s="52"/>
       <c r="M107" s="52"/>
       <c r="N107" s="52" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="O107" s="52"/>
       <c r="P107" s="52"/>
@@ -40994,7 +41178,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B109">
         <v>2481</v>
@@ -41020,7 +41204,48 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>321</v>
+        <v>317</v>
+      </c>
+      <c r="B110">
+        <v>860</v>
+      </c>
+      <c r="C110">
+        <v>3460</v>
+      </c>
+      <c r="D110">
+        <v>3115</v>
+      </c>
+      <c r="E110">
+        <v>24826</v>
+      </c>
+      <c r="K110">
+        <v>460</v>
+      </c>
+      <c r="N110">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>318</v>
+      </c>
+      <c r="B111">
+        <v>904</v>
+      </c>
+      <c r="C111">
+        <v>3680</v>
+      </c>
+      <c r="D111">
+        <v>3285</v>
+      </c>
+      <c r="E111">
+        <v>26119.4</v>
+      </c>
+      <c r="K111">
+        <v>504</v>
+      </c>
+      <c r="N111">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -41073,11 +41298,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617BFE3A-5538-4FC4-A07C-C660CA12141D}">
-  <dimension ref="A1:M363"/>
+  <dimension ref="A1:M370"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A363" sqref="A363"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A370" sqref="A370:I370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41107,7 +41332,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
@@ -41117,7 +41342,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>129</v>
@@ -41126,7 +41351,7 @@
         <v>232</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -41134,7 +41359,7 @@
         <v>107</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C2" s="8">
         <v>200</v>
@@ -41222,7 +41447,7 @@
         <v>107</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C6" s="8">
         <f>(D6*E6)</f>
@@ -41244,7 +41469,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
@@ -41286,7 +41511,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C9" s="8">
         <v>200</v>
@@ -41374,7 +41599,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C13" s="8">
         <f>(D13*E13)</f>
@@ -41396,7 +41621,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
@@ -41438,7 +41663,7 @@
         <v>113</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C16" s="8">
         <v>200</v>
@@ -41526,7 +41751,7 @@
         <v>113</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C20" s="8">
         <f>(D20*E20)</f>
@@ -41548,7 +41773,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
@@ -41590,7 +41815,7 @@
         <v>131</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C23" s="8">
         <v>200</v>
@@ -41678,7 +41903,7 @@
         <v>131</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C27" s="8">
         <f>(D27*E27)</f>
@@ -41700,7 +41925,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
@@ -41742,7 +41967,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C30" s="8">
         <v>200</v>
@@ -41830,7 +42055,7 @@
         <v>134</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C34" s="8">
         <f>(D34*E34)</f>
@@ -41852,7 +42077,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2">
@@ -41908,7 +42133,7 @@
         <v>138</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C38" s="8">
         <v>200</v>
@@ -41996,7 +42221,7 @@
         <v>138</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C42" s="8">
         <f>(D42*E42)</f>
@@ -42018,7 +42243,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
@@ -42060,7 +42285,7 @@
         <v>142</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C45" s="8">
         <v>200</v>
@@ -42148,7 +42373,7 @@
         <v>142</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C49" s="8">
         <f>(D49*E49)</f>
@@ -42170,7 +42395,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2">
@@ -42212,7 +42437,7 @@
         <v>145</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C52" s="8">
         <v>200</v>
@@ -42300,7 +42525,7 @@
         <v>145</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C56" s="8">
         <f>(D56*E56)</f>
@@ -42322,7 +42547,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2">
@@ -42364,7 +42589,7 @@
         <v>149</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C59" s="8">
         <v>200</v>
@@ -42452,7 +42677,7 @@
         <v>149</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C63" s="8">
         <f>(D63*E63)</f>
@@ -42474,7 +42699,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2">
@@ -42516,7 +42741,7 @@
         <v>153</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C66" s="8">
         <v>200</v>
@@ -42604,7 +42829,7 @@
         <v>153</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C70" s="8">
         <f>(D70*E70)</f>
@@ -42626,7 +42851,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2">
@@ -42668,7 +42893,7 @@
         <v>156</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C73" s="8">
         <v>200</v>
@@ -42756,7 +42981,7 @@
         <v>156</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C77" s="8">
         <f>(D77*E77)</f>
@@ -42778,7 +43003,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2">
@@ -42834,7 +43059,7 @@
         <v>158</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C81" s="8">
         <v>200</v>
@@ -42922,7 +43147,7 @@
         <v>158</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C85" s="8">
         <f>(D85*E85)</f>
@@ -42944,7 +43169,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="2">
@@ -42986,7 +43211,7 @@
         <v>160</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C88" s="8">
         <v>200</v>
@@ -43074,7 +43299,7 @@
         <v>160</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C92" s="8">
         <f>(D92*E92)</f>
@@ -43096,7 +43321,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="2">
@@ -43138,7 +43363,7 @@
         <v>162</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C95" s="8">
         <v>200</v>
@@ -43226,7 +43451,7 @@
         <v>162</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C99" s="8">
         <f>(D99*E99)</f>
@@ -43248,7 +43473,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="2">
@@ -43290,7 +43515,7 @@
         <v>163</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C102" s="8">
         <v>200</v>
@@ -43378,7 +43603,7 @@
         <v>163</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C106" s="8">
         <f>(D106*E106)</f>
@@ -43400,7 +43625,7 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="2">
@@ -43442,7 +43667,7 @@
         <v>165</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C109" s="8">
         <v>200</v>
@@ -43530,7 +43755,7 @@
         <v>165</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C113" s="8">
         <f>(D113*E113)</f>
@@ -43552,7 +43777,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="2">
@@ -43594,7 +43819,7 @@
         <v>167</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C116" s="8">
         <v>200</v>
@@ -43682,7 +43907,7 @@
         <v>167</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C120" s="8">
         <f>(D120*E120)</f>
@@ -43704,7 +43929,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="2">
@@ -43760,7 +43985,7 @@
         <v>169</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C124" s="8">
         <v>200</v>
@@ -43848,7 +44073,7 @@
         <v>169</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C128" s="8">
         <f>(D128*E128)</f>
@@ -43870,7 +44095,7 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="2">
@@ -43912,7 +44137,7 @@
         <v>170</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C131" s="8">
         <v>200</v>
@@ -44000,7 +44225,7 @@
         <v>170</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C135" s="8">
         <f>(D135*E135)</f>
@@ -44022,7 +44247,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="2">
@@ -44064,7 +44289,7 @@
         <v>171</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C138" s="8">
         <v>200</v>
@@ -44152,7 +44377,7 @@
         <v>171</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C142" s="8">
         <f>(D142*E142)</f>
@@ -44174,7 +44399,7 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="2">
@@ -44216,7 +44441,7 @@
         <v>175</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C145" s="8">
         <v>200</v>
@@ -44304,7 +44529,7 @@
         <v>175</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C149" s="8">
         <f>(D149*E149)</f>
@@ -44326,7 +44551,7 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="2">
@@ -44368,7 +44593,7 @@
         <v>180</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C152" s="8">
         <v>200</v>
@@ -44456,7 +44681,7 @@
         <v>180</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C156" s="8">
         <f>(D156*E156)</f>
@@ -44478,7 +44703,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="2">
@@ -44520,7 +44745,7 @@
         <v>181</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C159" s="8">
         <v>200</v>
@@ -44608,7 +44833,7 @@
         <v>181</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C163" s="8">
         <f>(D163*E163)</f>
@@ -44630,7 +44855,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B164" s="8"/>
       <c r="C164" s="2">
@@ -44686,7 +44911,7 @@
         <v>183</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C167" s="8">
         <v>200</v>
@@ -44774,7 +44999,7 @@
         <v>183</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C171" s="8">
         <f>(D171*E171)</f>
@@ -44796,7 +45021,7 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B172" s="8"/>
       <c r="C172" s="2">
@@ -44838,7 +45063,7 @@
         <v>185</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C174" s="8">
         <v>200</v>
@@ -44926,7 +45151,7 @@
         <v>185</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C178" s="8">
         <f>(D178*E178)</f>
@@ -44948,7 +45173,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B179" s="8"/>
       <c r="C179" s="2">
@@ -44990,7 +45215,7 @@
         <v>186</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C181" s="8">
         <v>200</v>
@@ -45078,7 +45303,7 @@
         <v>186</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C185" s="8">
         <f>(D185*E185)</f>
@@ -45100,7 +45325,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="2">
@@ -45142,7 +45367,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C188" s="8">
         <v>200</v>
@@ -45230,7 +45455,7 @@
         <v>187</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C192" s="8">
         <f>(D192*E192)</f>
@@ -45252,7 +45477,7 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B193" s="8"/>
       <c r="C193" s="2">
@@ -45294,7 +45519,7 @@
         <v>188</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C195" s="8">
         <v>200</v>
@@ -45382,7 +45607,7 @@
         <v>188</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C199" s="8">
         <f>(D199*E199)</f>
@@ -45404,7 +45629,7 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B200" s="8"/>
       <c r="C200" s="2">
@@ -45446,7 +45671,7 @@
         <v>190</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C202" s="8">
         <v>200</v>
@@ -45534,7 +45759,7 @@
         <v>190</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C206" s="8">
         <f>(D206*E206)</f>
@@ -45556,7 +45781,7 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B207" s="8"/>
       <c r="C207" s="2">
@@ -45612,7 +45837,7 @@
         <v>191</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C210" s="8">
         <v>200</v>
@@ -45700,7 +45925,7 @@
         <v>191</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C214" s="8">
         <f>(D214*E214)</f>
@@ -45722,7 +45947,7 @@
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B215" s="8"/>
       <c r="C215" s="2">
@@ -45764,7 +45989,7 @@
         <v>192</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C217" s="8">
         <v>200</v>
@@ -45852,7 +46077,7 @@
         <v>192</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C221" s="8">
         <f>(D221*E221)</f>
@@ -45874,7 +46099,7 @@
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B222" s="8"/>
       <c r="C222" s="2">
@@ -45916,7 +46141,7 @@
         <v>193</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C224" s="8">
         <v>200</v>
@@ -46004,7 +46229,7 @@
         <v>193</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C228" s="8">
         <f>(D228*E228)</f>
@@ -46026,7 +46251,7 @@
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B229" s="8"/>
       <c r="C229" s="2">
@@ -46068,7 +46293,7 @@
         <v>194</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C231" s="8">
         <v>200</v>
@@ -46156,7 +46381,7 @@
         <v>194</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C235" s="8">
         <f>(D235*E235)</f>
@@ -46178,7 +46403,7 @@
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B236" s="8"/>
       <c r="C236" s="2">
@@ -46220,7 +46445,7 @@
         <v>195</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C238" s="8">
         <v>200</v>
@@ -46308,7 +46533,7 @@
         <v>195</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C242" s="8">
         <f>(D242*E242)</f>
@@ -46330,7 +46555,7 @@
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B243" s="8"/>
       <c r="C243" s="2">
@@ -46372,7 +46597,7 @@
         <v>199</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C245" s="8">
         <v>200</v>
@@ -46460,7 +46685,7 @@
         <v>199</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C249" s="8">
         <f>(D249*E249)</f>
@@ -46482,7 +46707,7 @@
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B250" s="8"/>
       <c r="C250" s="2">
@@ -46538,7 +46763,7 @@
         <v>19</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C253" s="8">
         <v>200</v>
@@ -46626,7 +46851,7 @@
         <v>19</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C257" s="8">
         <f>(D257*E257)</f>
@@ -46648,7 +46873,7 @@
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B258" s="8"/>
       <c r="C258" s="2">
@@ -46690,7 +46915,7 @@
         <v>20</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C260" s="8">
         <v>200</v>
@@ -46778,7 +47003,7 @@
         <v>20</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C264" s="8">
         <f>(D264*E264)</f>
@@ -46800,7 +47025,7 @@
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B265" s="8"/>
       <c r="C265" s="2">
@@ -46839,10 +47064,10 @@
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C267" s="8">
         <v>200</v>
@@ -46863,7 +47088,7 @@
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B268" s="8" t="s">
         <v>121</v>
@@ -46887,7 +47112,7 @@
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B269" s="8" t="s">
         <v>73</v>
@@ -46907,7 +47132,7 @@
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B270" s="8" t="s">
         <v>122</v>
@@ -46927,10 +47152,10 @@
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C271" s="8">
         <f>(D271*E271)</f>
@@ -46952,7 +47177,7 @@
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B272" s="8"/>
       <c r="C272" s="2">
@@ -46991,10 +47216,10 @@
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C274" s="8">
         <v>200</v>
@@ -47015,7 +47240,7 @@
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B275" s="8" t="s">
         <v>121</v>
@@ -47039,7 +47264,7 @@
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B276" s="8" t="s">
         <v>73</v>
@@ -47059,7 +47284,7 @@
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B277" s="8" t="s">
         <v>122</v>
@@ -47079,10 +47304,10 @@
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C278" s="8">
         <f>(D278*E278)</f>
@@ -47104,7 +47329,7 @@
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A279" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B279" s="8"/>
       <c r="C279" s="2">
@@ -47143,10 +47368,10 @@
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A281" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C281" s="8">
         <v>200</v>
@@ -47167,7 +47392,7 @@
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B282" s="8" t="s">
         <v>121</v>
@@ -47191,7 +47416,7 @@
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A283" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B283" s="8" t="s">
         <v>73</v>
@@ -47211,7 +47436,7 @@
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B284" s="8" t="s">
         <v>122</v>
@@ -47231,10 +47456,10 @@
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A285" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C285" s="8">
         <f>(D285*E285)</f>
@@ -47256,7 +47481,7 @@
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B286" s="8"/>
       <c r="C286" s="2">
@@ -47294,10 +47519,10 @@
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C288" s="8">
         <v>200</v>
@@ -47322,7 +47547,7 @@
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A289" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B289" s="8" t="s">
         <v>121</v>
@@ -47350,7 +47575,7 @@
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B290" s="8" t="s">
         <v>73</v>
@@ -47374,7 +47599,7 @@
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A291" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B291" s="8" t="s">
         <v>122</v>
@@ -47394,10 +47619,10 @@
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C292" s="8">
         <f>(D292*E292)</f>
@@ -47419,7 +47644,7 @@
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A293" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B293" s="8"/>
       <c r="C293" s="2">
@@ -47444,7 +47669,7 @@
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B294" s="8"/>
       <c r="C294" s="2"/>
@@ -47487,7 +47712,7 @@
         <v>176</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C296" s="8">
         <v>200</v>
@@ -47603,7 +47828,7 @@
         <v>176</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C301" s="8">
         <f>(D301*E301)</f>
@@ -47625,7 +47850,7 @@
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B302" s="8"/>
       <c r="C302" s="2">
@@ -47704,7 +47929,7 @@
     </row>
     <row r="306" spans="1:13" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B306" s="15"/>
       <c r="C306" s="13">
@@ -47866,7 +48091,7 @@
         <v>177</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C314" s="8">
         <f>(D314*E314)</f>
@@ -47888,7 +48113,7 @@
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A315" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B315" s="8"/>
       <c r="C315" s="2">
@@ -48026,7 +48251,7 @@
         <v>220</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C321" s="8">
         <f>(D321*E321)</f>
@@ -48048,7 +48273,7 @@
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B322" s="8"/>
       <c r="C322" s="2">
@@ -48110,7 +48335,7 @@
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A325" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B325" t="s">
         <v>73</v>
@@ -48127,7 +48352,7 @@
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A326" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B326" t="s">
         <v>122</v>
@@ -48138,7 +48363,7 @@
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B327" t="s">
         <v>234</v>
@@ -48149,7 +48374,7 @@
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B328" t="s">
         <v>236</v>
@@ -48160,10 +48385,10 @@
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A329" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B329" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C329">
         <f>(D329*E329)</f>
@@ -48178,7 +48403,7 @@
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C330" s="2">
         <f>SUM(C325:C329)</f>
@@ -48206,7 +48431,7 @@
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A332" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B332" t="s">
         <v>73</v>
@@ -48223,7 +48448,7 @@
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A333" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B333" t="s">
         <v>122</v>
@@ -48240,7 +48465,7 @@
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A334" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B334" t="s">
         <v>234</v>
@@ -48251,7 +48476,7 @@
     </row>
     <row r="335" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A335" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B335" t="s">
         <v>236</v>
@@ -48262,10 +48487,10 @@
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B336" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C336">
         <f>(D336*E336)</f>
@@ -48280,7 +48505,7 @@
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C337" s="2">
         <f>SUM(C332:C336)</f>
@@ -48309,7 +48534,7 @@
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B339" t="s">
         <v>73</v>
@@ -48326,7 +48551,7 @@
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B340" t="s">
         <v>122</v>
@@ -48335,7 +48560,7 @@
         <v>250</v>
       </c>
       <c r="G340" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H340">
         <v>2000</v>
@@ -48343,7 +48568,7 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B341" t="s">
         <v>234</v>
@@ -48352,7 +48577,7 @@
         <v>250</v>
       </c>
       <c r="G341" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H341">
         <v>350</v>
@@ -48360,7 +48585,7 @@
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B342" t="s">
         <v>236</v>
@@ -48377,10 +48602,10 @@
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B343" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C343" s="8">
         <f>(D343*E343)</f>
@@ -48401,7 +48626,7 @@
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C344" s="2">
         <f>SUM(C339:C343)</f>
@@ -48430,7 +48655,7 @@
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B346" t="s">
         <v>73</v>
@@ -48447,7 +48672,7 @@
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B347" t="s">
         <v>122</v>
@@ -48464,7 +48689,7 @@
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B348" t="s">
         <v>234</v>
@@ -48481,7 +48706,7 @@
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B349" t="s">
         <v>236</v>
@@ -48492,10 +48717,10 @@
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B350" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C350">
         <f>(D350*E350)</f>
@@ -48510,7 +48735,7 @@
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C351" s="2">
         <f>SUM(C346:C350)</f>
@@ -48538,7 +48763,7 @@
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A353" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B353" t="s">
         <v>73</v>
@@ -48555,10 +48780,10 @@
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A354" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B354" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C354">
         <f>(D354*E354)</f>
@@ -48573,7 +48798,7 @@
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A355" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C355" s="2">
         <f>SUM(C353:C354)</f>
@@ -48612,7 +48837,7 @@
     </row>
     <row r="358" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B358" t="s">
         <v>73</v>
@@ -48629,7 +48854,7 @@
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A359" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B359" t="s">
         <v>122</v>
@@ -48646,10 +48871,10 @@
     </row>
     <row r="360" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A360" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B360" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C360">
         <f>(D360*E360)</f>
@@ -48664,7 +48889,7 @@
     </row>
     <row r="361" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A361" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C361" s="2">
         <f>SUM(C358:C360)</f>
@@ -48692,8 +48917,127 @@
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A363" s="2" t="s">
-        <v>321</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="B363" t="s">
+        <v>73</v>
+      </c>
+      <c r="C363">
+        <v>250</v>
+      </c>
+      <c r="G363" t="s">
+        <v>125</v>
+      </c>
+      <c r="H363">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A364" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B364" t="s">
+        <v>297</v>
+      </c>
+      <c r="C364">
+        <f>(D364*E364)</f>
+        <v>2021</v>
+      </c>
+      <c r="D364">
+        <v>860</v>
+      </c>
+      <c r="E364">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A365" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C365" s="2">
+        <f>SUM(C363:C364)</f>
+        <v>2271</v>
+      </c>
+      <c r="H365" s="2">
+        <v>750</v>
+      </c>
+      <c r="I365" s="2">
+        <f>(C365+H365)</f>
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A366" s="29"/>
+      <c r="B366" s="34"/>
+      <c r="C366" s="34"/>
+      <c r="D366" s="34"/>
+      <c r="E366" s="34"/>
+      <c r="F366" s="34"/>
+      <c r="G366" s="34"/>
+      <c r="H366" s="34"/>
+      <c r="I366" s="34"/>
+    </row>
+    <row r="367" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A367" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B367" t="s">
+        <v>73</v>
+      </c>
+      <c r="C367">
+        <v>250</v>
+      </c>
+      <c r="G367" t="s">
+        <v>125</v>
+      </c>
+      <c r="H367">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A368" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B368" t="s">
+        <v>297</v>
+      </c>
+      <c r="C368">
+        <f>(D368*E368)</f>
+        <v>2124.4</v>
+      </c>
+      <c r="D368">
+        <v>904</v>
+      </c>
+      <c r="E368">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A369" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C369" s="2">
+        <f>SUM(C367:C368)</f>
+        <v>2374.4</v>
+      </c>
+      <c r="H369" s="2">
+        <v>750</v>
+      </c>
+      <c r="I369" s="2">
+        <f>(C369+H369)</f>
+        <v>3124.4</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A370" s="29"/>
+      <c r="B370" s="34"/>
+      <c r="C370" s="34"/>
+      <c r="D370" s="34"/>
+      <c r="E370" s="34"/>
+      <c r="F370" s="34"/>
+      <c r="G370" s="34"/>
+      <c r="H370" s="34"/>
+      <c r="I370" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -48703,10 +49047,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD1A8C-99DF-4166-8097-144C71FF7489}">
-  <dimension ref="A1:BB12"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="BD11" sqref="BD11"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -48714,17 +49058,14 @@
     <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>222</v>
       </c>
@@ -48739,71 +49080,53 @@
       <c r="H1" s="46"/>
       <c r="I1" s="46"/>
       <c r="J1" s="26"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="57" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
       <c r="O1" s="24"/>
-      <c r="P1" s="47" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="U1" s="49" t="s">
+      <c r="P1" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Z1" s="50" t="s">
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="U1" s="50" t="s">
         <v>238</v>
       </c>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AE1" s="58" t="s">
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Z1" s="55" t="s">
         <v>239</v>
       </c>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AJ1" s="55" t="s">
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AE1" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AO1" s="54" t="s">
-        <v>241</v>
-      </c>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AT1" s="55" t="s">
-        <v>250</v>
-      </c>
-      <c r="AU1" s="55"/>
-      <c r="AV1" s="55"/>
-      <c r="AW1" s="55"/>
-      <c r="AY1" s="57" t="s">
-        <v>251</v>
-      </c>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="57"/>
-      <c r="BB1" s="57"/>
-    </row>
-    <row r="2" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AJ1" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+    </row>
+    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>221</v>
@@ -48812,10 +49135,10 @@
         <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>221</v>
@@ -48824,10 +49147,10 @@
         <v>59</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>221</v>
@@ -48836,10 +49159,10 @@
         <v>59</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>221</v>
@@ -48848,10 +49171,10 @@
         <v>59</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>221</v>
@@ -48860,10 +49183,10 @@
         <v>59</v>
       </c>
       <c r="AA2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>221</v>
@@ -48872,10 +49195,10 @@
         <v>59</v>
       </c>
       <c r="AF2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>221</v>
@@ -48884,52 +49207,16 @@
         <v>59</v>
       </c>
       <c r="AK2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="AM2" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AO2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>38000</v>
       </c>
@@ -48960,89 +49247,56 @@
         <f>(L3-M3)</f>
         <v>16297</v>
       </c>
-      <c r="P3" s="1">
-        <v>44404</v>
-      </c>
+      <c r="P3" s="1"/>
       <c r="Q3">
-        <v>20300</v>
+        <v>10650</v>
+      </c>
+      <c r="R3">
+        <v>5000</v>
       </c>
       <c r="S3">
         <f>(Q3-R3)</f>
-        <v>20300</v>
-      </c>
-      <c r="U3" s="1"/>
+        <v>5650</v>
+      </c>
       <c r="V3">
-        <v>10650</v>
-      </c>
-      <c r="W3">
-        <v>5000</v>
+        <v>28947</v>
       </c>
       <c r="X3">
         <f>(V3-W3)</f>
-        <v>5650</v>
+        <v>28947</v>
       </c>
       <c r="AA3">
-        <v>28947</v>
+        <v>35737</v>
+      </c>
+      <c r="AB3">
+        <v>10000</v>
       </c>
       <c r="AC3">
         <f>(AA3-AB3)</f>
-        <v>28947</v>
+        <v>25737</v>
       </c>
       <c r="AE3" s="1">
-        <v>44400</v>
+        <v>44399</v>
       </c>
       <c r="AF3">
-        <v>35499</v>
-      </c>
-      <c r="AG3">
-        <v>30000</v>
+        <v>23310</v>
       </c>
       <c r="AH3">
         <f>(AF3-AG3)</f>
-        <v>5499</v>
+        <v>23310</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>44403</v>
       </c>
       <c r="AK3">
-        <v>35737</v>
-      </c>
-      <c r="AL3">
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="AM3">
         <f>(AK3-AL3)</f>
-        <v>25737</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>44399</v>
-      </c>
-      <c r="AP3">
-        <v>23310</v>
-      </c>
-      <c r="AR3">
-        <f>(AP3-AQ3)</f>
-        <v>23310</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>44403</v>
-      </c>
-      <c r="AU3">
-        <v>1050</v>
-      </c>
-      <c r="AW3">
-        <f>(AU3-AV3)</f>
-        <v>1050</v>
-      </c>
-      <c r="AY3" s="1">
-        <v>44403</v>
-      </c>
-      <c r="AZ3">
         <v>9000</v>
       </c>
-      <c r="BB3">
-        <f>(AZ3-BA3)</f>
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44402</v>
       </c>
@@ -49076,58 +49330,38 @@
         <f t="shared" ref="N4:N9" si="1">(L4-M4+N3)</f>
         <v>34758</v>
       </c>
-      <c r="P4" s="1">
-        <v>44408</v>
-      </c>
-      <c r="R4">
+      <c r="U4" s="1">
+        <v>44403</v>
+      </c>
+      <c r="V4">
+        <v>26628</v>
+      </c>
+      <c r="X4">
+        <f>(V4-W4+X3)</f>
+        <v>55575</v>
+      </c>
+      <c r="AB4">
         <v>10000</v>
       </c>
-      <c r="S4">
-        <f>(Q4-R4+S3)</f>
-        <v>10300</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>44403</v>
-      </c>
-      <c r="AA4">
-        <v>26628</v>
-      </c>
       <c r="AC4">
-        <f>(AA4-AB4+AC3)</f>
-        <v>55575</v>
-      </c>
-      <c r="AL4">
-        <v>10000</v>
-      </c>
-      <c r="AM4">
-        <f>(AM3+AK4-AL4)</f>
+        <f>(AC3+AA4-AB4)</f>
         <v>15737</v>
       </c>
-      <c r="AO4" s="1">
+      <c r="AE4" s="1">
         <v>44404</v>
       </c>
-      <c r="AP4">
+      <c r="AF4">
         <v>18875</v>
       </c>
-      <c r="AQ4">
+      <c r="AG4">
         <v>25000</v>
       </c>
-      <c r="AR4">
-        <f>(AP4-AQ4+AR3)</f>
+      <c r="AH4">
+        <f>(AF4-AG4+AH3)</f>
         <v>17185</v>
       </c>
-      <c r="AT4" s="1">
-        <v>44404</v>
-      </c>
-      <c r="AU4">
-        <v>10950</v>
-      </c>
-      <c r="AW4">
-        <f>(AU4-AV4+AW3)</f>
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44403</v>
       </c>
@@ -49161,58 +49395,38 @@
         <f t="shared" si="1"/>
         <v>41758</v>
       </c>
-      <c r="P5" t="s">
-        <v>318</v>
-      </c>
-      <c r="R5">
-        <v>1300</v>
-      </c>
-      <c r="S5">
-        <f>(Q5-R5+S4)</f>
-        <v>9000</v>
+      <c r="U5" s="1">
+        <v>44404</v>
+      </c>
+      <c r="V5">
+        <v>18039</v>
+      </c>
+      <c r="X5">
+        <f>(V5-W5+X4)</f>
+        <v>73614</v>
       </c>
       <c r="Z5" s="1">
-        <v>44404</v>
+        <v>44403</v>
       </c>
       <c r="AA5">
-        <v>18039</v>
+        <v>28100</v>
       </c>
       <c r="AC5">
-        <f>(AA5-AB5+AC4)</f>
-        <v>73614</v>
-      </c>
-      <c r="AJ5" s="1">
-        <v>44403</v>
-      </c>
-      <c r="AK5">
-        <v>28100</v>
-      </c>
-      <c r="AM5">
-        <f>(AM4+AK5-AL5)</f>
+        <f>(AC4+AA5-AB5)</f>
         <v>43837</v>
       </c>
-      <c r="AO5" s="1">
+      <c r="AE5" s="1">
         <v>44408</v>
       </c>
-      <c r="AQ5">
+      <c r="AG5">
         <v>10000</v>
       </c>
-      <c r="AR5">
-        <f>(AP5-AQ5+AR4)</f>
+      <c r="AH5">
+        <f>(AF5-AG5+AH4)</f>
         <v>7185</v>
       </c>
-      <c r="AT5" s="1">
-        <v>44408</v>
-      </c>
-      <c r="AV5">
-        <v>5000</v>
-      </c>
-      <c r="AW5">
-        <f>(AU5-AV5+AW4)</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44404</v>
       </c>
@@ -49246,44 +49460,44 @@
         <f t="shared" si="1"/>
         <v>31093</v>
       </c>
+      <c r="U6" s="1">
+        <v>44405</v>
+      </c>
+      <c r="V6">
+        <v>21750</v>
+      </c>
+      <c r="W6">
+        <v>20000</v>
+      </c>
+      <c r="X6">
+        <f>(V6-W6+X5)</f>
+        <v>75364</v>
+      </c>
       <c r="Z6" s="1">
-        <v>44405</v>
+        <v>44404</v>
       </c>
       <c r="AA6">
-        <v>21750</v>
+        <v>13400</v>
       </c>
       <c r="AB6">
-        <v>20000</v>
+        <v>13400</v>
       </c>
       <c r="AC6">
         <f>(AA6-AB6+AC5)</f>
-        <v>75364</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>44404</v>
-      </c>
-      <c r="AK6">
-        <v>13400</v>
-      </c>
-      <c r="AL6">
-        <v>13400</v>
-      </c>
-      <c r="AM6">
-        <f>(AK6-AL6+AM5)</f>
         <v>43837</v>
       </c>
-      <c r="AO6" s="1">
+      <c r="AE6" s="1">
         <v>44409</v>
       </c>
-      <c r="AP6">
+      <c r="AF6">
         <v>9325</v>
       </c>
-      <c r="AR6">
-        <f>(AP6-AQ6+AR5)</f>
+      <c r="AH6">
+        <f>(AF6-AG6+AH5)</f>
         <v>16510</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44405</v>
       </c>
@@ -49317,13 +49531,33 @@
         <f t="shared" si="1"/>
         <v>45093</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="U7" s="1">
+        <v>44411</v>
+      </c>
+      <c r="V7">
+        <v>32900</v>
+      </c>
+      <c r="X7">
+        <f>(V7-W7+X6)</f>
+        <v>108264</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>316</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>44411</v>
+      </c>
+      <c r="AG7">
+        <v>10000</v>
+      </c>
+      <c r="AH7">
+        <f>(AF7-AG7+AH6)</f>
+        <v>6510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F8" s="1">
         <v>44405</v>
@@ -49349,7 +49583,7 @@
         <v>47043</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="F9" s="1">
         <v>44406</v>
       </c>
@@ -49374,7 +49608,7 @@
         <v>46093</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="F10" s="1">
         <v>44409</v>
       </c>
@@ -49396,7 +49630,7 @@
         <v>70093</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="K11" s="1">
         <v>44406</v>
       </c>
@@ -49408,7 +49642,7 @@
         <v>30093</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="K12" s="1">
         <v>44409</v>
       </c>
@@ -49420,19 +49654,28 @@
         <v>59093</v>
       </c>
     </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="K13" s="1">
+        <v>44411</v>
+      </c>
+      <c r="L13">
+        <v>11900</v>
+      </c>
+      <c r="N13">
+        <f>(L13-M13+N12)</f>
+        <v>70993</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="8">
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="K1:N1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="P1:S1"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AY1:BB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49462,7 +49705,7 @@
         <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>120</v>
@@ -49471,25 +49714,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>221</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -49523,10 +49766,10 @@
         <v>44385</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D3">
         <v>714</v>
@@ -49552,7 +49795,7 @@
         <v>44385</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4">
         <v>2720</v>
@@ -49603,7 +49846,7 @@
         <v>44388</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7">
         <v>2720</v>
@@ -49649,12 +49892,12 @@
         <v>-5289.15</v>
       </c>
       <c r="K9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s">
         <v>125</v>
@@ -49683,7 +49926,7 @@
         <v>44390</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D11">
         <v>340</v>
@@ -49709,7 +49952,7 @@
         <v>44390</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D12">
         <v>510</v>
@@ -49735,7 +49978,7 @@
         <v>44391</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D13">
         <v>612</v>
@@ -49761,7 +50004,7 @@
         <v>44391</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D14">
         <v>510</v>
@@ -49813,7 +50056,7 @@
         <v>44392</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D16">
         <v>306</v>
@@ -49846,7 +50089,7 @@
         <v>1657.1500000000015</v>
       </c>
       <c r="K17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -49887,7 +50130,7 @@
         <v>-15146.849999999999</v>
       </c>
       <c r="K19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -49895,7 +50138,7 @@
         <v>44394</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D20">
         <v>510</v>
@@ -49921,7 +50164,7 @@
         <v>44394</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D21">
         <v>714</v>
@@ -49947,7 +50190,7 @@
         <v>44394</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D22">
         <v>510</v>
@@ -49973,7 +50216,7 @@
         <v>44394</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D23">
         <v>731</v>
@@ -49999,7 +50242,7 @@
         <v>44395</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D24">
         <v>561</v>
@@ -50025,7 +50268,7 @@
         <v>44395</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D25">
         <v>910</v>
@@ -50051,7 +50294,7 @@
         <v>44395</v>
       </c>
       <c r="B26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D26">
         <v>731</v>
@@ -50077,7 +50320,7 @@
         <v>44398</v>
       </c>
       <c r="B27" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D27">
         <v>680</v>
@@ -50103,7 +50346,7 @@
         <v>44398</v>
       </c>
       <c r="B28" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D28">
         <v>425</v>
@@ -50129,7 +50372,7 @@
         <v>44398</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D29">
         <v>1020</v>
@@ -50155,7 +50398,7 @@
         <v>44398</v>
       </c>
       <c r="B30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D30">
         <v>731</v>
@@ -50181,7 +50424,7 @@
         <v>44398</v>
       </c>
       <c r="B31" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D31">
         <v>561</v>
@@ -50207,7 +50450,7 @@
         <v>44398</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D32">
         <v>306</v>
@@ -50233,7 +50476,7 @@
         <v>44398</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D33">
         <v>408</v>
@@ -50259,7 +50502,7 @@
         <v>44398</v>
       </c>
       <c r="B34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D34">
         <v>1156</v>
@@ -50285,10 +50528,10 @@
         <v>44399</v>
       </c>
       <c r="B35" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C35" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D35">
         <v>510</v>
@@ -50314,7 +50557,7 @@
         <v>44399</v>
       </c>
       <c r="B36" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D36">
         <v>204</v>
@@ -50337,13 +50580,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D37">
         <v>340</v>
@@ -50369,10 +50612,10 @@
         <v>44399</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D38">
         <v>85</v>
@@ -50398,10 +50641,10 @@
         <v>44399</v>
       </c>
       <c r="B39" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D39">
         <v>221</v>
@@ -50427,7 +50670,7 @@
         <v>44399</v>
       </c>
       <c r="B40" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D40">
         <v>680</v>
@@ -50453,10 +50696,10 @@
         <v>44399</v>
       </c>
       <c r="B41" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C41" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D41">
         <v>408</v>
@@ -50482,7 +50725,7 @@
         <v>44399</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D42">
         <v>748</v>
@@ -50508,7 +50751,7 @@
         <v>44399</v>
       </c>
       <c r="B43" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D43">
         <v>629</v>
@@ -50534,7 +50777,7 @@
         <v>44399</v>
       </c>
       <c r="B44" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D44">
         <v>799</v>
@@ -50560,10 +50803,10 @@
         <v>44400</v>
       </c>
       <c r="B45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C45" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D45">
         <v>255</v>
@@ -50589,7 +50832,7 @@
         <v>44400</v>
       </c>
       <c r="B46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C46" t="s">
         <v>223</v>
@@ -50618,10 +50861,10 @@
         <v>44400</v>
       </c>
       <c r="B47" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C47" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D47">
         <v>748</v>
@@ -50654,7 +50897,7 @@
         <v>12067.750000000004</v>
       </c>
       <c r="K48" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
@@ -50662,10 +50905,10 @@
         <v>44401</v>
       </c>
       <c r="B49" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D49">
         <v>408</v>
@@ -50691,7 +50934,7 @@
         <v>44401</v>
       </c>
       <c r="B50" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D50">
         <v>459</v>
@@ -50717,10 +50960,10 @@
         <v>44401</v>
       </c>
       <c r="B51" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D51">
         <v>799</v>
@@ -50746,7 +50989,7 @@
         <v>44401</v>
       </c>
       <c r="B52" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D52">
         <v>1020</v>
@@ -50772,7 +51015,7 @@
         <v>44402</v>
       </c>
       <c r="B53" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D53">
         <v>119</v>
@@ -50798,10 +51041,10 @@
         <v>44402</v>
       </c>
       <c r="B54" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C54" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D54">
         <v>272</v>
@@ -50827,7 +51070,7 @@
         <v>44402</v>
       </c>
       <c r="B55" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D55">
         <v>612</v>
@@ -50853,10 +51096,10 @@
         <v>44402</v>
       </c>
       <c r="B56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D56">
         <v>714</v>
@@ -50882,7 +51125,7 @@
         <v>44402</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D57">
         <v>901</v>
@@ -50908,7 +51151,7 @@
         <v>44402</v>
       </c>
       <c r="B58" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D58">
         <v>204</v>
@@ -50941,7 +51184,7 @@
         <v>-16533.449999999993</v>
       </c>
       <c r="K59" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>